<commit_message>
remove hit dhit and other config
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fish\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="194">
   <si>
     <t>stop</t>
   </si>
@@ -328,14 +328,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Hit/=0.4;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit*=0.4;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.Atk/=0.1;o.Def/=0.1;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -376,24 +368,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.DHit/=0.5;</t>
-  </si>
-  <si>
-    <t>o.DHit*=0.5;</t>
-  </si>
-  <si>
-    <t>o.Hit/=0.25;o.DHit/=0.25;</t>
-  </si>
-  <si>
-    <t>o.Hit*=0.25;o.DHit*=0.25;</t>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;o.DHit*=0.2;</t>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;o.DHit/=0.2;</t>
-  </si>
-  <si>
     <t>打分</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -526,10 +500,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Hit*=0.1;o.DHit*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>atk1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -550,14 +520,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Hit/=0.1;o.DHit/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit/=0.1;o.DHit/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>全属性下降20%</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -749,11 +711,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.2;o.Def/=0.2;o.Hit/=0.2;o.DHit/=0.2;o.Spd/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;o.Def*=0.2;o.Hit*=0.2;o.DHit*=0.2;o.Spd*=0.2;</t>
+    <t>o.Atk/=0.2;o.Def/=0.2;o.Spd/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;o.Def*=0.2;o.Spd*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2095,72 +2065,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FF81FF81"/>
       <color rgb="FF0066FF"/>
@@ -2217,7 +2121,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2499,10 +2403,10 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2546,10 +2450,10 @@
         <v>53</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>60</v>
@@ -2566,7 +2470,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -2584,10 +2488,10 @@
         <v>82</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>47</v>
@@ -2622,10 +2526,10 @@
         <v>83</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>59</v>
@@ -2636,17 +2540,13 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>103</v>
-      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="14">
         <v>0</v>
@@ -2655,10 +2555,10 @@
         <v>69</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="K4" s="13">
         <v>300</v>
@@ -2694,7 +2594,7 @@
         <v>78</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="K5" s="13">
         <v>300</v>
@@ -2730,7 +2630,7 @@
         <v>75</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="K6" s="13">
         <v>1000</v>
@@ -2750,10 +2650,10 @@
         <v>63</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14">
@@ -2763,10 +2663,10 @@
         <v>69</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="K7" s="13">
         <v>400</v>
@@ -2798,7 +2698,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="K8" s="13">
         <v>200</v>
@@ -2821,16 +2721,16 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="K9" s="13">
         <v>950</v>
@@ -2864,7 +2764,7 @@
         <v>81</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="K10" s="13">
         <v>200</v>
@@ -2884,10 +2784,10 @@
         <v>63</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="14">
@@ -2897,10 +2797,10 @@
         <v>69</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="K11" s="13">
         <v>600</v>
@@ -2929,10 +2829,10 @@
         <v>69</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K12" s="13">
         <v>2000</v>
@@ -2954,7 +2854,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G13" s="14">
         <v>0</v>
@@ -2963,10 +2863,10 @@
         <v>69</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="K13" s="13">
         <v>200</v>
@@ -2985,12 +2885,8 @@
       <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>91</v>
-      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="14">
         <v>0</v>
@@ -3002,7 +2898,7 @@
         <v>76</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="K14" s="13">
         <v>400</v>
@@ -3025,16 +2921,16 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="K15" s="13">
         <v>2500</v>
@@ -3056,7 +2952,7 @@
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G16" s="14">
         <v>0</v>
@@ -3065,10 +2961,10 @@
         <v>69</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="K16" s="13">
         <v>200</v>
@@ -3077,7 +2973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="22.5">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>56000014</v>
       </c>
@@ -3087,12 +2983,8 @@
       <c r="C17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>105</v>
-      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="14">
         <v>0</v>
@@ -3104,7 +2996,7 @@
         <v>77</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="K17" s="13">
         <v>500</v>
@@ -3126,7 +3018,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G18" s="14">
         <v>1</v>
@@ -3135,10 +3027,10 @@
         <v>69</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="K18" s="13">
         <v>250</v>
@@ -3152,10 +3044,10 @@
         <v>56000016</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -3167,10 +3059,10 @@
         <v>69</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="K19" s="13">
         <v>500</v>
@@ -3202,7 +3094,7 @@
         <v>45</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K20" s="13">
         <v>120</v>
@@ -3222,23 +3114,23 @@
         <v>63</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="K21" s="13">
         <v>1500</v>
@@ -3261,16 +3153,16 @@
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K22" s="13">
         <v>1500</v>
@@ -3279,7 +3171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="33.75">
+    <row r="23" spans="1:12" ht="22.5">
       <c r="A23">
         <v>56000021</v>
       </c>
@@ -3290,10 +3182,10 @@
         <v>63</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="14">
@@ -3303,10 +3195,10 @@
         <v>69</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="K23" s="16">
         <v>2000</v>
@@ -3338,7 +3230,7 @@
         <v>39</v>
       </c>
       <c r="J24" s="31" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="K24" s="13">
         <v>4000</v>
@@ -3347,7 +3239,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="22.5">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>56000023</v>
       </c>
@@ -3358,10 +3250,10 @@
         <v>64</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="14">
@@ -3374,7 +3266,7 @@
         <v>74</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="K25" s="13">
         <v>600</v>
@@ -3388,16 +3280,16 @@
         <v>56000101</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="14">
@@ -3407,16 +3299,16 @@
         <v>69</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K26" s="13">
         <v>400</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="22.5">
@@ -3424,16 +3316,16 @@
         <v>56000102</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="14">
@@ -3443,16 +3335,16 @@
         <v>69</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K27" s="13">
         <v>800</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="22.5">
@@ -3460,16 +3352,16 @@
         <v>56000111</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="14">
@@ -3479,34 +3371,30 @@
         <v>69</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K28" s="13">
         <v>400</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="22.5">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>56000121</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>147</v>
-      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="14">
         <v>0</v>
@@ -3515,34 +3403,30 @@
         <v>69</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K29" s="13">
         <v>200</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="22.5">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>56000131</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>141</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="14">
         <v>0</v>
@@ -3551,16 +3435,16 @@
         <v>69</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K30" s="13">
         <v>200</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3589,119 +3473,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
         <v>151</v>
       </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" t="s">
-        <v>162</v>
-      </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
         <v>157</v>
       </c>
-      <c r="B3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" t="s">
-        <v>168</v>
-      </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monster attr add hit dhit crt so on as stable attr relative to atk and hp
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="184">
   <si>
     <t>stop</t>
   </si>
@@ -308,30 +308,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Spd/=0.3;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Spd*=0.3;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Def/=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Def*=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.AddHp(-o.Hp*0.1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.1;o.Def/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法攻击</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -356,14 +336,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Def*=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Def/=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法被治疗，每回合减少5%生命</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -380,14 +352,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Ats-=3;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Ats+=3;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>降低30%攻击速度</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -412,10 +376,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.Def*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.AddHp(-o.Atk*0.3);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -440,10 +400,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk*=0.1;o.Def*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提高10%攻击和10%防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -452,14 +408,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk*=0.2;o.Def*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;o.Def/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提高20%攻击和20%防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -472,14 +420,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.1;o.Def/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.1;o.Def*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>降低10%攻击和10%防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -711,19 +651,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.2;o.Def/=0.2;o.Spd/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;o.Def*=0.2;o.Spd*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.Atk*=0.2;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2403,10 +2363,10 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2450,10 +2410,10 @@
         <v>53</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>60</v>
@@ -2470,7 +2430,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -2488,10 +2448,10 @@
         <v>82</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>47</v>
@@ -2526,10 +2486,10 @@
         <v>83</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>59</v>
@@ -2540,7 +2500,7 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>63</v>
@@ -2555,10 +2515,10 @@
         <v>69</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="K4" s="13">
         <v>300</v>
@@ -2577,12 +2537,8 @@
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>86</v>
-      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="14">
         <v>0</v>
@@ -2594,7 +2550,7 @@
         <v>78</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="K5" s="13">
         <v>300</v>
@@ -2613,12 +2569,8 @@
       <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>88</v>
-      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="14">
         <v>0</v>
@@ -2630,7 +2582,7 @@
         <v>75</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="K6" s="13">
         <v>1000</v>
@@ -2650,10 +2602,10 @@
         <v>63</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14">
@@ -2663,10 +2615,10 @@
         <v>69</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="K7" s="13">
         <v>400</v>
@@ -2698,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="K8" s="13">
         <v>200</v>
@@ -2721,16 +2673,16 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="K9" s="13">
         <v>950</v>
@@ -2752,7 +2704,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G10" s="14">
         <v>0</v>
@@ -2764,7 +2716,7 @@
         <v>81</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="K10" s="13">
         <v>200</v>
@@ -2783,12 +2735,8 @@
       <c r="C11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>104</v>
-      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="14">
         <v>0</v>
@@ -2797,10 +2745,10 @@
         <v>69</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="K11" s="13">
         <v>600</v>
@@ -2829,10 +2777,10 @@
         <v>69</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="K12" s="13">
         <v>2000</v>
@@ -2854,7 +2802,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>111</v>
+        <v>183</v>
       </c>
       <c r="G13" s="14">
         <v>0</v>
@@ -2863,10 +2811,10 @@
         <v>69</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="K13" s="13">
         <v>200</v>
@@ -2898,7 +2846,7 @@
         <v>76</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="K14" s="13">
         <v>400</v>
@@ -2921,16 +2869,16 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="K15" s="13">
         <v>2500</v>
@@ -2952,7 +2900,7 @@
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G16" s="14">
         <v>0</v>
@@ -2961,10 +2909,10 @@
         <v>69</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="K16" s="13">
         <v>200</v>
@@ -2996,7 +2944,7 @@
         <v>77</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="K17" s="13">
         <v>500</v>
@@ -3018,7 +2966,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="G18" s="14">
         <v>1</v>
@@ -3027,10 +2975,10 @@
         <v>69</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="K18" s="13">
         <v>250</v>
@@ -3044,10 +2992,10 @@
         <v>56000016</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -3059,10 +3007,10 @@
         <v>69</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="K19" s="13">
         <v>500</v>
@@ -3094,7 +3042,7 @@
         <v>45</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K20" s="13">
         <v>120</v>
@@ -3113,24 +3061,20 @@
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>98</v>
-      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="K21" s="13">
         <v>1500</v>
@@ -3153,16 +3097,16 @@
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="K22" s="13">
         <v>1500</v>
@@ -3171,7 +3115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="22.5">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>56000021</v>
       </c>
@@ -3182,10 +3126,10 @@
         <v>63</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="14">
@@ -3195,10 +3139,10 @@
         <v>69</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="K23" s="16">
         <v>2000</v>
@@ -3230,7 +3174,7 @@
         <v>39</v>
       </c>
       <c r="J24" s="31" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="K24" s="13">
         <v>4000</v>
@@ -3250,10 +3194,10 @@
         <v>64</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="14">
@@ -3266,7 +3210,7 @@
         <v>74</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="K25" s="13">
         <v>600</v>
@@ -3275,21 +3219,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="22.5">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>56000101</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="14">
@@ -3299,33 +3243,33 @@
         <v>69</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K26" s="13">
         <v>400</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="22.5">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>56000102</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="14">
@@ -3335,33 +3279,33 @@
         <v>69</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K27" s="13">
         <v>800</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="22.5">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>56000111</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>127</v>
+        <v>182</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="14">
@@ -3371,16 +3315,16 @@
         <v>69</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K28" s="13">
         <v>400</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -3388,7 +3332,7 @@
         <v>56000121</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>61</v>
@@ -3403,16 +3347,16 @@
         <v>69</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K29" s="13">
         <v>200</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -3420,10 +3364,10 @@
         <v>56000131</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -3435,16 +3379,16 @@
         <v>69</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="K30" s="13">
         <v>200</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3473,119 +3417,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#13 add immune group attr replace attratk
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -19,8 +19,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>real</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1.生命
+2.意志
+3.肉体
+4.元素
+5.联动</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="187">
   <si>
     <t>stop</t>
   </si>
@@ -684,6 +724,18 @@
   </si>
   <si>
     <t>o.AddHp(-1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>免疫组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -691,7 +743,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -891,6 +943,21 @@
       <charset val="134"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="54">
     <fill>
@@ -1638,7 +1705,34 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2050,24 +2144,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:L30" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:L30"/>
-  <sortState ref="A4:K30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:M30"/>
+  <sortState ref="A4:M30">
     <sortCondition ref="A3:A30"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Type" dataDxfId="9"/>
-    <tableColumn id="15" name="OnAdd" dataDxfId="8"/>
-    <tableColumn id="14" name="OnRemove" dataDxfId="7"/>
-    <tableColumn id="17" name="OnRound" dataDxfId="6"/>
-    <tableColumn id="8" name="Effect" dataDxfId="5"/>
-    <tableColumn id="9" name="EndOnHit" dataDxfId="4"/>
-    <tableColumn id="11" name="GetDescript" dataDxfId="3"/>
-    <tableColumn id="6" name="Color" dataDxfId="2"/>
-    <tableColumn id="4" name="Mark" dataDxfId="1"/>
-    <tableColumn id="13" name="Icon" dataDxfId="0"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" name="Type" dataDxfId="10"/>
+    <tableColumn id="5" name="Group" dataDxfId="0"/>
+    <tableColumn id="15" name="OnAdd" dataDxfId="9"/>
+    <tableColumn id="14" name="OnRemove" dataDxfId="8"/>
+    <tableColumn id="17" name="OnRound" dataDxfId="7"/>
+    <tableColumn id="8" name="Effect" dataDxfId="6"/>
+    <tableColumn id="9" name="EndOnHit" dataDxfId="5"/>
+    <tableColumn id="11" name="GetDescript" dataDxfId="4"/>
+    <tableColumn id="6" name="Color" dataDxfId="3"/>
+    <tableColumn id="4" name="Mark" dataDxfId="2"/>
+    <tableColumn id="13" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2359,29 +2454,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="6.75" customWidth="1"/>
-    <col min="4" max="6" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="6.375" customWidth="1"/>
-    <col min="9" max="9" width="34.75" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
-    <col min="11" max="11" width="6.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="7" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="6.375" customWidth="1"/>
+    <col min="10" max="10" width="34.75" customWidth="1"/>
+    <col min="11" max="11" width="12.75" customWidth="1"/>
+    <col min="12" max="12" width="6.125" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -2392,34 +2487,37 @@
         <v>50</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -2430,34 +2528,37 @@
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
@@ -2467,35 +2568,38 @@
       <c r="C3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>56000001</v>
       </c>
@@ -2505,29 +2609,32 @@
       <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="14">
+      <c r="G4" s="15"/>
+      <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="K4" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="K4" s="13">
+      <c r="L4" s="13">
         <v>300</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>56000002</v>
       </c>
@@ -2537,29 +2644,32 @@
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="14">
+      <c r="G5" s="15"/>
+      <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="K5" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="13">
         <v>300</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>56000003</v>
       </c>
@@ -2569,29 +2679,32 @@
       <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="14">
+      <c r="G6" s="15"/>
+      <c r="H6" s="14">
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="K6" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="K6" s="13">
+      <c r="L6" s="13">
         <v>1000</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>56000004</v>
       </c>
@@ -2601,33 +2714,36 @@
       <c r="C7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="14">
+      <c r="G7" s="15"/>
+      <c r="H7" s="14">
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="K7" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="K7" s="13">
+      <c r="L7" s="13">
         <v>400</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>56000005</v>
       </c>
@@ -2637,29 +2753,32 @@
       <c r="C8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="K8" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K8" s="13">
+      <c r="L8" s="13">
         <v>200</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>56000006</v>
       </c>
@@ -2669,29 +2788,32 @@
       <c r="C9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="K9" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="K9" s="13">
+      <c r="L9" s="13">
         <v>950</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>56000007</v>
       </c>
@@ -2701,31 +2823,34 @@
       <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="14">
+      <c r="H10" s="14">
         <v>0</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="K10" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="K10" s="13">
+      <c r="L10" s="13">
         <v>200</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>56000008</v>
       </c>
@@ -2735,29 +2860,32 @@
       <c r="C11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="4">
+        <v>4</v>
+      </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="14">
+      <c r="G11" s="15"/>
+      <c r="H11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="K11" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="K11" s="13">
+      <c r="L11" s="13">
         <v>600</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>56000009</v>
       </c>
@@ -2767,29 +2895,32 @@
       <c r="C12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="14">
+      <c r="G12" s="15"/>
+      <c r="H12" s="14">
         <v>2</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="K12" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="K12" s="13">
+      <c r="L12" s="13">
         <v>2000</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>56000010</v>
       </c>
@@ -2799,31 +2930,34 @@
       <c r="C13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="14">
+      <c r="H13" s="14">
         <v>0</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="K13" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="K13" s="13">
+      <c r="L13" s="13">
         <v>200</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>56000011</v>
       </c>
@@ -2833,29 +2967,32 @@
       <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="14">
+      <c r="G14" s="15"/>
+      <c r="H14" s="14">
         <v>0</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="K14" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="K14" s="13">
+      <c r="L14" s="13">
         <v>400</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>56000012</v>
       </c>
@@ -2865,29 +3002,32 @@
       <c r="C15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="15"/>
+      <c r="H15" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="K15" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="K15" s="13">
+      <c r="L15" s="13">
         <v>2500</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>56000013</v>
       </c>
@@ -2897,31 +3037,34 @@
       <c r="C16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="14">
+      <c r="H16" s="14">
         <v>0</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="J16" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="K16" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="K16" s="13">
+      <c r="L16" s="13">
         <v>200</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>56000014</v>
       </c>
@@ -2931,29 +3074,32 @@
       <c r="C17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="14">
+      <c r="G17" s="15"/>
+      <c r="H17" s="14">
         <v>0</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="K17" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="K17" s="13">
+      <c r="L17" s="13">
         <v>500</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>56000015</v>
       </c>
@@ -2963,31 +3109,34 @@
       <c r="C18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G18" s="14">
+      <c r="H18" s="14">
         <v>1</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="J18" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="K18" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="K18" s="13">
+      <c r="L18" s="13">
         <v>250</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>56000016</v>
       </c>
@@ -2997,29 +3146,32 @@
       <c r="C19" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="14">
+      <c r="G19" s="15"/>
+      <c r="H19" s="14">
         <v>5</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="J19" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="K19" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="K19" s="13">
+      <c r="L19" s="13">
         <v>500</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>56000017</v>
       </c>
@@ -3029,29 +3181,32 @@
       <c r="C20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="14">
+      <c r="G20" s="15"/>
+      <c r="H20" s="14">
         <v>4</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K20" s="13">
+      <c r="L20" s="13">
         <v>120</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>56000018</v>
       </c>
@@ -3061,29 +3216,32 @@
       <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="4">
+        <v>4</v>
+      </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="15"/>
+      <c r="H21" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="J21" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="K21" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="K21" s="13">
+      <c r="L21" s="13">
         <v>1500</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>56000019</v>
       </c>
@@ -3093,29 +3251,32 @@
       <c r="C22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="15"/>
+      <c r="H22" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="K22" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="K22" s="13">
+      <c r="L22" s="13">
         <v>1500</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>56000021</v>
       </c>
@@ -3125,33 +3286,36 @@
       <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="F23" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="14">
+      <c r="G23" s="15"/>
+      <c r="H23" s="14">
         <v>0</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="24" t="s">
+      <c r="K23" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="K23" s="16">
+      <c r="L23" s="16">
         <v>2000</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>56000022</v>
       </c>
@@ -3161,29 +3325,32 @@
       <c r="C24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="14">
+      <c r="G24" s="15"/>
+      <c r="H24" s="14">
         <v>102</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="K24" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="K24" s="13">
+      <c r="L24" s="13">
         <v>4000</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="M24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>56000023</v>
       </c>
@@ -3193,33 +3360,36 @@
       <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="14">
+      <c r="G25" s="15"/>
+      <c r="H25" s="14">
         <v>101</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="J25" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J25" s="34" t="s">
+      <c r="K25" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="K25" s="13">
+      <c r="L25" s="13">
         <v>600</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="M25" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>56000101</v>
       </c>
@@ -3229,33 +3399,36 @@
       <c r="C26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="F26" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="14">
+      <c r="G26" s="15"/>
+      <c r="H26" s="14">
         <v>0</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="J26" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K26" s="13">
+      <c r="L26" s="13">
         <v>400</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="M26" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>56000102</v>
       </c>
@@ -3265,33 +3438,36 @@
       <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="F27" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="14">
+      <c r="G27" s="15"/>
+      <c r="H27" s="14">
         <v>0</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="J27" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K27" s="13">
+      <c r="L27" s="13">
         <v>800</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="M27" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>56000111</v>
       </c>
@@ -3301,33 +3477,36 @@
       <c r="C28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="F28" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="14">
+      <c r="G28" s="15"/>
+      <c r="H28" s="14">
         <v>0</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="J28" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K28" s="13">
+      <c r="L28" s="13">
         <v>400</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>56000121</v>
       </c>
@@ -3337,29 +3516,32 @@
       <c r="C29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="15"/>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="14">
+      <c r="G29" s="15"/>
+      <c r="H29" s="14">
         <v>0</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K29" s="13">
+      <c r="L29" s="13">
         <v>200</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>56000131</v>
       </c>
@@ -3369,25 +3551,28 @@
       <c r="C30" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="14">
+      <c r="G30" s="15"/>
+      <c r="H30" s="14">
         <v>0</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="J30" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K30" s="13">
+      <c r="L30" s="13">
         <v>200</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="M30" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3395,8 +3580,9 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
remove some useless interface of IMonster; implement the canmove attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -55,6 +55,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+        NoCure = 1,
+        NoAttack = 2,
+        NoTile = 3,
+        NoAuro = 4,
+        NoSkill = 5,
+        NoMove = 6,
+        Tile = 101,
+        Rebel = 102,
+        Chaos = 103,</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -400,10 +434,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>降低30%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>静止</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -736,6 +766,10 @@
   </si>
   <si>
     <t>Group</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位无法移动</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1706,33 +1740,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1993,6 +2000,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -2153,16 +2187,16 @@
     <tableColumn id="1" name="Id" dataDxfId="12"/>
     <tableColumn id="2" name="Name" dataDxfId="11"/>
     <tableColumn id="3" name="Type" dataDxfId="10"/>
-    <tableColumn id="5" name="Group" dataDxfId="0"/>
-    <tableColumn id="15" name="OnAdd" dataDxfId="9"/>
-    <tableColumn id="14" name="OnRemove" dataDxfId="8"/>
-    <tableColumn id="17" name="OnRound" dataDxfId="7"/>
-    <tableColumn id="8" name="Effect" dataDxfId="6"/>
-    <tableColumn id="9" name="EndOnHit" dataDxfId="5"/>
-    <tableColumn id="11" name="GetDescript" dataDxfId="4"/>
-    <tableColumn id="6" name="Color" dataDxfId="3"/>
-    <tableColumn id="4" name="Mark" dataDxfId="2"/>
-    <tableColumn id="13" name="Icon" dataDxfId="1"/>
+    <tableColumn id="5" name="Group" dataDxfId="9"/>
+    <tableColumn id="15" name="OnAdd" dataDxfId="8"/>
+    <tableColumn id="14" name="OnRemove" dataDxfId="7"/>
+    <tableColumn id="17" name="OnRound" dataDxfId="6"/>
+    <tableColumn id="8" name="Effect" dataDxfId="5"/>
+    <tableColumn id="9" name="EndOnHit" dataDxfId="4"/>
+    <tableColumn id="11" name="GetDescript" dataDxfId="3"/>
+    <tableColumn id="6" name="Color" dataDxfId="2"/>
+    <tableColumn id="4" name="Mark" dataDxfId="1"/>
+    <tableColumn id="13" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2461,19 +2495,19 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="3" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="7" width="15.625" customWidth="1"/>
-    <col min="9" max="9" width="6.375" customWidth="1"/>
-    <col min="10" max="10" width="34.75" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="6.125" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="3" max="4" width="6.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="34.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2487,7 +2521,7 @@
         <v>50</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>71</v>
@@ -2508,7 +2542,7 @@
         <v>53</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>93</v>
@@ -2528,7 +2562,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>91</v>
@@ -2549,7 +2583,7 @@
         <v>82</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>94</v>
@@ -2569,7 +2603,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>70</v>
@@ -2590,7 +2624,7 @@
         <v>83</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>95</v>
@@ -2604,7 +2638,7 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>63</v>
@@ -2616,16 +2650,16 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>69</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>98</v>
+        <v>186</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L4" s="13">
         <v>300</v>
@@ -2660,7 +2694,7 @@
         <v>78</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L5" s="13">
         <v>300</v>
@@ -2695,7 +2729,7 @@
         <v>75</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L6" s="13">
         <v>1000</v>
@@ -2718,10 +2752,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
@@ -2731,10 +2765,10 @@
         <v>69</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L7" s="13">
         <v>400</v>
@@ -2769,7 +2803,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L8" s="13">
         <v>200</v>
@@ -2801,10 +2835,10 @@
         <v>69</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L9" s="13">
         <v>950</v>
@@ -2813,7 +2847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="21.6">
       <c r="A10">
         <v>56000007</v>
       </c>
@@ -2841,7 +2875,7 @@
         <v>81</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L10" s="13">
         <v>200</v>
@@ -2876,7 +2910,7 @@
         <v>96</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L11" s="13">
         <v>600</v>
@@ -2911,7 +2945,7 @@
         <v>86</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L12" s="13">
         <v>2000</v>
@@ -2936,7 +2970,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H13" s="14">
         <v>0</v>
@@ -2945,10 +2979,10 @@
         <v>69</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L13" s="13">
         <v>200</v>
@@ -2983,7 +3017,7 @@
         <v>76</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L14" s="13">
         <v>400</v>
@@ -3018,7 +3052,7 @@
         <v>89</v>
       </c>
       <c r="K15" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L15" s="13">
         <v>2500</v>
@@ -3027,7 +3061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" ht="21.6">
       <c r="A16">
         <v>56000013</v>
       </c>
@@ -3043,7 +3077,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="14">
         <v>0</v>
@@ -3052,10 +3086,10 @@
         <v>69</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L16" s="13">
         <v>200</v>
@@ -3090,7 +3124,7 @@
         <v>77</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L17" s="13">
         <v>500</v>
@@ -3099,7 +3133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" ht="21.6">
       <c r="A18">
         <v>56000015</v>
       </c>
@@ -3127,7 +3161,7 @@
         <v>92</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L18" s="13">
         <v>250</v>
@@ -3141,10 +3175,10 @@
         <v>56000016</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
@@ -3162,7 +3196,7 @@
         <v>88</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L19" s="13">
         <v>500</v>
@@ -3197,7 +3231,7 @@
         <v>45</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L20" s="13">
         <v>120</v>
@@ -3229,10 +3263,10 @@
         <v>69</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L21" s="13">
         <v>1500</v>
@@ -3264,10 +3298,10 @@
         <v>68</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L22" s="13">
         <v>1500</v>
@@ -3290,10 +3324,10 @@
         <v>1</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
@@ -3303,10 +3337,10 @@
         <v>69</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L23" s="16">
         <v>2000</v>
@@ -3341,7 +3375,7 @@
         <v>39</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L24" s="13">
         <v>4000</v>
@@ -3364,10 +3398,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>175</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>176</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="14">
@@ -3380,7 +3414,7 @@
         <v>74</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L25" s="13">
         <v>600</v>
@@ -3394,7 +3428,7 @@
         <v>56000101</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>61</v>
@@ -3403,10 +3437,10 @@
         <v>0</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="14">
@@ -3416,16 +3450,16 @@
         <v>69</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L26" s="13">
         <v>400</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -3433,7 +3467,7 @@
         <v>56000102</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>61</v>
@@ -3442,10 +3476,10 @@
         <v>0</v>
       </c>
       <c r="E27" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>180</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="14">
@@ -3455,16 +3489,16 @@
         <v>69</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L27" s="13">
         <v>800</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3472,19 +3506,19 @@
         <v>56000111</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
       </c>
       <c r="E28" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>182</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="14">
@@ -3494,16 +3528,16 @@
         <v>69</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L28" s="13">
         <v>400</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -3511,7 +3545,7 @@
         <v>56000121</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>61</v>
@@ -3529,16 +3563,16 @@
         <v>69</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L29" s="13">
         <v>200</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3546,10 +3580,10 @@
         <v>56000131</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -3564,16 +3598,16 @@
         <v>69</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L30" s="13">
         <v>200</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3595,127 +3629,127 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="6" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="6" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>128</v>
-      </c>
-      <c r="F1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
         <v>136</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>137</v>
-      </c>
-      <c r="F2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" t="s">
         <v>140</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>141</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>142</v>
-      </c>
-      <c r="F3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
         <v>144</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>145</v>
-      </c>
-      <c r="F4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
         <v>142</v>
       </c>
-      <c r="D5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" t="s">
         <v>146</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>147</v>
-      </c>
-      <c r="F6" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #34 finish anger; refine the skill burst code
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="188">
   <si>
     <t>stop</t>
   </si>
@@ -207,15 +207,6 @@
     <t>aging</t>
   </si>
   <si>
-    <t>背叛</t>
-  </si>
-  <si>
-    <t>rebel</t>
-  </si>
-  <si>
-    <t>目标会攻击己方</t>
-  </si>
-  <si>
     <t>地形</t>
   </si>
   <si>
@@ -302,119 +293,458 @@
     <t>ta</t>
   </si>
   <si>
+    <t>EndOnHit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnRemove</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高20%攻击和20%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低50%防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低40%命中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低25%命中和回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低30%速度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnRound</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少10%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormatStringDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetDescript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuffEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Hp*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法使用技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击，无法使用技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;103</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuffEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法被治疗，每回合减少5%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mark</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低30%攻击速度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Hp*0.05);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>静止</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法被治疗，攻击时有20%几率击中自身</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少30%防御的生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Atk*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少30%攻击的生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低20%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高10%攻击和10%防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高20%攻击和20%防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>na</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低10%攻击和10%防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高10%命中和10%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低10%命中和10%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atkr1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitr1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性下降20%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-100%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-80%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-60%</t>
+  </si>
+  <si>
+    <t>全属性-40%</t>
+  </si>
+  <si>
+    <t>全属性-20%</t>
+  </si>
+  <si>
+    <t>5回</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4回</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3回</t>
+  </si>
+  <si>
+    <t>2回</t>
+  </si>
+  <si>
+    <t>1回</t>
+  </si>
+  <si>
+    <t>1600分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200分</t>
+  </si>
+  <si>
+    <t>800分</t>
+  </si>
+  <si>
+    <t>400分</t>
+  </si>
+  <si>
+    <t>1600分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1280分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>960分</t>
+  </si>
+  <si>
+    <t>640分</t>
+  </si>
+  <si>
+    <t>320分</t>
+  </si>
+  <si>
+    <t>720分</t>
+  </si>
+  <si>
+    <t>480分</t>
+  </si>
+  <si>
+    <t>240分</t>
+  </si>
+  <si>
+    <t>160分</t>
+  </si>
+  <si>
+    <t>80分</t>
+  </si>
+  <si>
+    <t>封印</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>ns</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EndOnHit</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>移除时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnRemove</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高20%攻击和20%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低50%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低40%命中</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低25%命中和回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低30%速度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnRound</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少10%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FormatStringDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetDescript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuffEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Hp*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法使用技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击，无法使用技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;103</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuffEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法被治疗，每回合减少5%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打分</t>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>色彩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,255,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>156,0,24</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>128,0,128</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>200,100,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>196,196,196</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52,52,52</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,255,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,102,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>239,125,141</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,255,204</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,255,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,102,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,102,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>129,255,129</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击和使用技能，但会提高50%防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击和使用技能，但受到攻击后状态解除</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>免疫组</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -422,354 +752,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Mark</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低30%攻击速度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Hp*0.05);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>静止</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法被治疗，攻击时有20%几率击中自身</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少30%防御的生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Atk*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少30%攻击的生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低20%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高10%攻击和10%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防+2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高20%攻击和20%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>na</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低10%攻击和10%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>命避+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高10%命中和10%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低10%命中和10%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>命避-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atkr1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hitr1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性下降20%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-100%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2000分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-80%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-60%</t>
-  </si>
-  <si>
-    <t>全属性-40%</t>
-  </si>
-  <si>
-    <t>全属性-20%</t>
-  </si>
-  <si>
-    <t>5回</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>4回</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3回</t>
-  </si>
-  <si>
-    <t>2回</t>
-  </si>
-  <si>
-    <t>1回</t>
-  </si>
-  <si>
-    <t>1600分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1200分</t>
-  </si>
-  <si>
-    <t>800分</t>
-  </si>
-  <si>
-    <t>400分</t>
-  </si>
-  <si>
-    <t>1600分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1280分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>960分</t>
-  </si>
-  <si>
-    <t>640分</t>
-  </si>
-  <si>
-    <t>320分</t>
-  </si>
-  <si>
-    <t>720分</t>
-  </si>
-  <si>
-    <t>480分</t>
-  </si>
-  <si>
-    <t>240分</t>
-  </si>
-  <si>
-    <t>160分</t>
-  </si>
-  <si>
-    <t>80分</t>
-  </si>
-  <si>
-    <t>封印</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ns</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>色彩</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,0,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,255,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,0,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>156,0,24</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>128,0,128</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>200,100,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>196,196,196</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52,52,52</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,255,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,102,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>239,125,141</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,0,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,255,204</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,255,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,102,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,102,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>129,255,129</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击和使用技能，但会提高50%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击和使用技能，但受到攻击后状态解除</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>免疫组</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Group</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>单位无法移动</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激怒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ps</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>该单位目前被激怒了</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>193,7,65</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>anger</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -993,7 +1000,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="54">
+  <fills count="55">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1296,6 +1303,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81FF81"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC10741"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1588,7 +1601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1692,6 +1705,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="53" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="54" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2154,6 +2170,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC10741"/>
       <color rgb="FF81FF81"/>
       <color rgb="FF0066FF"/>
       <color rgb="FF000000"/>
@@ -2163,7 +2180,6 @@
       <color rgb="FFEF7D8D"/>
       <color rgb="FF006600"/>
       <color rgb="FFFFFF00"/>
-      <color rgb="FF343434"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2492,10 +2508,10 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2512,125 +2528,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="K1" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2638,10 +2654,10 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -2653,13 +2669,13 @@
         <v>6</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L4" s="13">
         <v>300</v>
@@ -2676,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -2688,13 +2704,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="L5" s="13">
         <v>300</v>
@@ -2711,7 +2727,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -2723,13 +2739,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L6" s="13">
         <v>1000</v>
@@ -2746,29 +2762,29 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L7" s="13">
         <v>400</v>
@@ -2785,7 +2801,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -2797,13 +2813,13 @@
         <v>9</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="L8" s="13">
         <v>200</v>
@@ -2820,7 +2836,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
@@ -2829,16 +2845,16 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L9" s="13">
         <v>950</v>
@@ -2855,7 +2871,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -2863,19 +2879,19 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H10" s="14">
         <v>0</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L10" s="13">
         <v>200</v>
@@ -2892,7 +2908,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -2904,13 +2920,13 @@
         <v>0</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="L11" s="13">
         <v>600</v>
@@ -2927,7 +2943,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4">
         <v>4</v>
@@ -2939,13 +2955,13 @@
         <v>2</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L12" s="13">
         <v>2000</v>
@@ -2962,7 +2978,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="4">
         <v>4</v>
@@ -2970,19 +2986,19 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H13" s="14">
         <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="L13" s="13">
         <v>200</v>
@@ -2999,7 +3015,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
@@ -3011,13 +3027,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L14" s="13">
         <v>400</v>
@@ -3034,7 +3050,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" s="4">
         <v>3</v>
@@ -3043,16 +3059,16 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K15" s="30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="L15" s="13">
         <v>2500</v>
@@ -3069,7 +3085,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -3077,19 +3093,19 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H16" s="14">
         <v>0</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L16" s="13">
         <v>200</v>
@@ -3106,7 +3122,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -3118,13 +3134,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L17" s="13">
         <v>500</v>
@@ -3141,7 +3157,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -3149,19 +3165,19 @@
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H18" s="14">
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L18" s="13">
         <v>250</v>
@@ -3175,10 +3191,10 @@
         <v>56000016</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
@@ -3190,19 +3206,19 @@
         <v>5</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L19" s="13">
         <v>500</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -3210,10 +3226,10 @@
         <v>56000017</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
@@ -3225,19 +3241,19 @@
         <v>4</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L20" s="13">
         <v>120</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -3248,7 +3264,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -3257,16 +3273,16 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L21" s="13">
         <v>1500</v>
@@ -3283,7 +3299,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" s="4">
         <v>2</v>
@@ -3292,16 +3308,16 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L22" s="13">
         <v>1500</v>
@@ -3318,29 +3334,29 @@
         <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
         <v>0</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L23" s="16">
         <v>2000</v>
@@ -3351,34 +3367,38 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>56000022</v>
+        <v>56000023</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>171</v>
+      </c>
       <c r="G24" s="15"/>
       <c r="H24" s="14">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="34" t="s">
         <v>167</v>
       </c>
       <c r="L24" s="13">
-        <v>4000</v>
+        <v>600</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>38</v>
@@ -3386,169 +3406,165 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
-        <v>56000023</v>
+        <v>56000101</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="14">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>171</v>
+        <v>103</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="L25" s="13">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26">
-        <v>56000101</v>
+        <v>56000102</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="14">
         <v>0</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L26" s="13">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27">
-        <v>56000102</v>
+        <v>56000111</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="14">
         <v>0</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L27" s="13">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
-        <v>56000111</v>
+        <v>56000121</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>181</v>
-      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="14">
         <v>0</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L28" s="13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29">
-        <v>56000121</v>
+        <v>56000131</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -3560,30 +3576,30 @@
         <v>0</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L29" s="13">
         <v>200</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30">
-        <v>56000131</v>
+        <v>56000201</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -3595,19 +3611,19 @@
         <v>0</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L30" s="13">
-        <v>200</v>
+        <v>185</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="L30" s="16">
+        <v>0</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3637,119 +3653,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" t="s">
-        <v>127</v>
-      </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
         <v>130</v>
       </c>
-      <c r="B3" t="s">
-        <v>134</v>
-      </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
       <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" t="s">
         <v>140</v>
       </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>144</v>
-      </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
         <v>142</v>
-      </c>
-      <c r="F5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
         <v>133</v>
       </c>
-      <c r="B6" t="s">
-        <v>137</v>
-      </c>
       <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" t="s">
         <v>142</v>
       </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" t="s">
-        <v>146</v>
-      </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish card Mycoron #32
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="184">
   <si>
     <t>stop</t>
   </si>
@@ -141,12 +141,6 @@
     <t>poison</t>
   </si>
   <si>
-    <t>冻伤</t>
-  </si>
-  <si>
-    <t>snow</t>
-  </si>
-  <si>
     <t>冰冻</t>
   </si>
   <si>
@@ -413,10 +407,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>降低30%攻击速度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.AddHp(-o.Hp*0.05);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -629,10 +619,6 @@
   </si>
   <si>
     <t>0,255,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100,255</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1000,7 +986,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="55">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1219,12 +1205,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0000FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6464FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1601,7 +1581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1653,25 +1633,25 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="42" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="42" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="43" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1689,25 +1669,22 @@
     <xf numFmtId="49" fontId="0" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="50" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="53" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="54" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2194,8 +2171,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A3:M30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:M29"/>
   <sortState ref="A4:M30">
     <sortCondition ref="A3:A30"/>
   </sortState>
@@ -2505,13 +2482,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2528,125 +2505,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="K1" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2654,10 +2631,10 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -2669,13 +2646,13 @@
         <v>6</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>160</v>
+        <v>178</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>156</v>
       </c>
       <c r="L4" s="13">
         <v>300</v>
@@ -2692,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -2704,13 +2681,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>159</v>
+        <v>72</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>155</v>
       </c>
       <c r="L5" s="13">
         <v>300</v>
@@ -2727,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -2739,13 +2716,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>158</v>
+        <v>69</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>154</v>
       </c>
       <c r="L6" s="13">
         <v>1000</v>
@@ -2762,29 +2739,29 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>161</v>
+        <v>96</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>157</v>
       </c>
       <c r="L7" s="13">
         <v>400</v>
@@ -2801,7 +2778,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -2813,13 +2790,13 @@
         <v>9</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="23" t="s">
-        <v>155</v>
+      <c r="K8" s="22" t="s">
+        <v>151</v>
       </c>
       <c r="L8" s="13">
         <v>200</v>
@@ -2836,7 +2813,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
@@ -2845,16 +2822,16 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>163</v>
+        <v>92</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="L9" s="13">
         <v>950</v>
@@ -2871,7 +2848,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -2879,19 +2856,19 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H10" s="14">
         <v>0</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>150</v>
+        <v>75</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="L10" s="13">
         <v>200</v>
@@ -2902,13 +2879,13 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
-        <v>56000008</v>
+        <v>56000009</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -2917,19 +2894,19 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>151</v>
+        <v>63</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>148</v>
       </c>
       <c r="L11" s="13">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>16</v>
@@ -2937,34 +2914,36 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
-        <v>56000009</v>
+        <v>56000010</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4">
         <v>4</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>174</v>
+      </c>
       <c r="H12" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="L12" s="13">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>18</v>
@@ -2972,36 +2951,34 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13">
-        <v>56000010</v>
+        <v>56000011</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="15" t="s">
-        <v>178</v>
-      </c>
+      <c r="G13" s="15"/>
       <c r="H13" s="14">
         <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>149</v>
+        <v>70</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>152</v>
       </c>
       <c r="L13" s="13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>20</v>
@@ -3009,13 +2986,13 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
-        <v>56000011</v>
+        <v>56000012</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
@@ -3023,178 +3000,178 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="14">
-        <v>0</v>
+      <c r="H14" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>156</v>
+        <v>63</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>158</v>
       </c>
       <c r="L14" s="13">
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="21.6">
       <c r="A15">
-        <v>56000012</v>
+        <v>56000013</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14" t="s">
-        <v>83</v>
+      <c r="G15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K15" s="30" t="s">
-        <v>162</v>
+        <v>63</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="L15" s="13">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21.6">
+    <row r="16" spans="1:13">
       <c r="A16">
-        <v>56000013</v>
+        <v>56000014</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="15" t="s">
-        <v>97</v>
-      </c>
+      <c r="G16" s="15"/>
       <c r="H16" s="14">
         <v>0</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L16" s="13">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" ht="21.6">
       <c r="A17">
-        <v>56000014</v>
+        <v>56000015</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="H17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>154</v>
+        <v>86</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="L17" s="13">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21.6">
+    <row r="18" spans="1:13">
       <c r="A18">
-        <v>56000015</v>
+        <v>56000016</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="15" t="s">
-        <v>93</v>
-      </c>
+      <c r="G18" s="15"/>
       <c r="H18" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>150</v>
+        <v>82</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>161</v>
       </c>
       <c r="L18" s="13">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <v>56000016</v>
+        <v>56000017</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>144</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
@@ -3203,19 +3180,19 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>165</v>
+        <v>63</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="L19" s="13">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>39</v>
@@ -3223,66 +3200,66 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <v>56000017</v>
+        <v>56000018</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="14">
-        <v>4</v>
+      <c r="H20" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>164</v>
       </c>
+      <c r="K20" s="24" t="s">
+        <v>153</v>
+      </c>
       <c r="L20" s="13">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
-        <v>56000018</v>
+        <v>56000019</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>157</v>
+        <v>62</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K21" s="32" t="s">
+        <v>162</v>
       </c>
       <c r="L21" s="13">
         <v>1500</v>
@@ -3293,34 +3270,38 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
-        <v>56000019</v>
+        <v>56000021</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="4">
-        <v>2</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>168</v>
+      </c>
       <c r="G22" s="15"/>
-      <c r="H22" s="14" t="s">
-        <v>83</v>
+      <c r="H22" s="14">
+        <v>0</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="K22" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="L22" s="13">
-        <v>1500</v>
+        <v>63</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="L22" s="16">
+        <v>2000</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>34</v>
@@ -3328,38 +3309,38 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23">
-        <v>56000021</v>
+        <v>56000023</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="L23" s="16">
-        <v>2000</v>
+        <v>68</v>
+      </c>
+      <c r="K23" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" s="13">
+        <v>600</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>36</v>
@@ -3367,169 +3348,165 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>56000023</v>
+        <v>56000101</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="14">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="34" t="s">
-        <v>167</v>
+        <v>100</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="L24" s="13">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
-        <v>56000101</v>
+        <v>56000102</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="14">
         <v>0</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L25" s="13">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26">
-        <v>56000102</v>
+        <v>56000111</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="14">
         <v>0</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>105</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L26" s="13">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27">
-        <v>56000111</v>
+        <v>56000121</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>106</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>177</v>
-      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="14">
         <v>0</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L27" s="13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
-        <v>56000121</v>
+        <v>56000131</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>109</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
@@ -3541,30 +3518,30 @@
         <v>0</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L28" s="13">
         <v>200</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29">
-        <v>56000131</v>
+        <v>56000201</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -3576,54 +3553,19 @@
         <v>0</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L29" s="13">
-        <v>200</v>
+        <v>181</v>
+      </c>
+      <c r="K29" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="L29" s="16">
+        <v>0</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30">
-        <v>56000201</v>
-      </c>
-      <c r="B30" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="14">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3653,119 +3595,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
         <v>135</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" t="s">
         <v>136</v>
       </c>
-      <c r="D4" t="s">
-        <v>139</v>
-      </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
         <v>137</v>
       </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
         <v>138</v>
       </c>
-      <c r="D6" t="s">
-        <v>141</v>
-      </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove some useless buff. keep some attr can change
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="171">
   <si>
     <t>stop</t>
   </si>
@@ -117,18 +117,6 @@
     <t>weak</t>
   </si>
   <si>
-    <t>贯通</t>
-  </si>
-  <si>
-    <t>tranfix</t>
-  </si>
-  <si>
-    <t>3;4</t>
-  </si>
-  <si>
-    <t>取消地形和光环支援</t>
-  </si>
-  <si>
     <t>混乱</t>
   </si>
   <si>
@@ -195,30 +183,12 @@
     <t>sleep</t>
   </si>
   <si>
-    <t>衰老</t>
-  </si>
-  <si>
-    <t>aging</t>
-  </si>
-  <si>
     <t>地形</t>
   </si>
   <si>
     <t>tile</t>
   </si>
   <si>
-    <t>saintmark</t>
-  </si>
-  <si>
-    <t>孤单</t>
-  </si>
-  <si>
-    <t>longly</t>
-  </si>
-  <si>
-    <t>无法获得支援效果</t>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -371,10 +341,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>无法使用技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法攻击，无法使用技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -503,10 +469,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>全属性下降20%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>全属性-100%</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -590,14 +552,6 @@
     <t>80分</t>
   </si>
   <si>
-    <t>封印</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ns</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -630,10 +584,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>200,100,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>100,100,100</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -670,10 +620,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>255,102,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0,102,255</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -695,10 +641,6 @@
   </si>
   <si>
     <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1010,7 +952,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="55">
+  <fills count="53">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1240,12 +1182,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC86400"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF646464"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1289,12 +1225,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1611,7 +1541,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1678,7 +1608,7 @@
     <xf numFmtId="49" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="42" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1696,25 +1626,19 @@
     <xf numFmtId="49" fontId="0" fillId="46" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="50" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="53" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
@@ -1732,7 +1656,7 @@
     <xf numFmtId="49" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="54" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2219,8 +2143,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A3:M30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:M26"/>
   <sortState ref="A4:M30">
     <sortCondition ref="A3:A30"/>
   </sortState>
@@ -2530,13 +2454,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2553,125 +2477,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>76</v>
-      </c>
       <c r="K3" s="12" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2679,10 +2603,10 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -2694,13 +2618,13 @@
         <v>6</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>155</v>
+        <v>160</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>140</v>
       </c>
       <c r="L4" s="13">
         <v>300</v>
@@ -2717,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -2729,13 +2653,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>154</v>
+        <v>61</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>139</v>
       </c>
       <c r="L5" s="13">
         <v>300</v>
@@ -2752,7 +2676,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -2764,13 +2688,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>153</v>
+        <v>58</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>138</v>
       </c>
       <c r="L6" s="13">
         <v>1000</v>
@@ -2787,29 +2711,29 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>156</v>
+        <v>84</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="L7" s="13">
         <v>400</v>
@@ -2820,34 +2744,34 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
-        <v>56000005</v>
+        <v>56000006</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="14" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>150</v>
+        <v>52</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="L8" s="13">
-        <v>200</v>
+        <v>950</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>8</v>
@@ -2855,157 +2779,157 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
-        <v>56000006</v>
+        <v>56000007</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14" t="s">
-        <v>83</v>
+      <c r="G9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="14">
+        <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>158</v>
+        <v>64</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="L9" s="13">
-        <v>950</v>
+        <v>200</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
-        <v>56000007</v>
+        <v>56000009</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="15" t="s">
-        <v>78</v>
-      </c>
+      <c r="G10" s="15"/>
       <c r="H10" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>146</v>
+        <v>52</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="L10" s="13">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
-        <v>56000009</v>
+        <v>56000010</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>156</v>
+      </c>
       <c r="H11" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>147</v>
+        <v>52</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="L11" s="13">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
-        <v>56000010</v>
+        <v>56000011</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15" t="s">
-        <v>173</v>
-      </c>
+      <c r="G12" s="15"/>
       <c r="H12" s="14">
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>145</v>
+        <v>59</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>136</v>
       </c>
       <c r="L12" s="13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13">
-        <v>56000011</v>
+        <v>56000012</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4">
         <v>3</v>
@@ -3013,642 +2937,498 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="14">
-        <v>0</v>
+      <c r="H13" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>151</v>
+        <v>52</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>142</v>
       </c>
       <c r="L13" s="13">
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
-        <v>56000012</v>
+        <v>56000013</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D14" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="14" t="s">
-        <v>80</v>
+      <c r="G14" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="29" t="s">
-        <v>157</v>
+        <v>52</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="L14" s="13">
-        <v>2500</v>
+        <v>200</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
-        <v>56000013</v>
+        <v>56000014</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15" t="s">
-        <v>93</v>
-      </c>
+      <c r="G15" s="15"/>
       <c r="H15" s="14">
         <v>0</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>148</v>
+        <v>60</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="L15" s="13">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
-        <v>56000014</v>
+        <v>56000015</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="H16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>149</v>
+        <v>74</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="L16" s="13">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
-        <v>56000015</v>
+        <v>56000018</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1</v>
+      <c r="G17" s="15"/>
+      <c r="H17" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>137</v>
       </c>
       <c r="L17" s="13">
-        <v>250</v>
+        <v>1500</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
-        <v>56000016</v>
+        <v>56000019</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>140</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="14">
-        <v>5</v>
+      <c r="H18" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" s="31" t="s">
-        <v>160</v>
+        <v>51</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>145</v>
       </c>
       <c r="L18" s="13">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <v>56000017</v>
+        <v>56000023</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4">
-        <v>5</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="14">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>159</v>
+        <v>52</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>146</v>
       </c>
       <c r="L19" s="13">
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <v>56000018</v>
+        <v>56000101</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4">
-        <v>4</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>154</v>
+      </c>
       <c r="G20" s="15"/>
-      <c r="H20" s="14" t="s">
-        <v>80</v>
+      <c r="H20" s="14">
+        <v>0</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>152</v>
+        <v>88</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="L20" s="13">
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
-        <v>56000019</v>
+        <v>56000102</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D21" s="4">
-        <v>2</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>153</v>
+      </c>
       <c r="G21" s="15"/>
-      <c r="H21" s="14" t="s">
-        <v>80</v>
+      <c r="H21" s="14">
+        <v>0</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>161</v>
+        <v>52</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="L21" s="13">
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
-        <v>56000021</v>
+        <v>56000111</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="14">
         <v>0</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="L22" s="16">
-        <v>2000</v>
+        <v>93</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L22" s="13">
+        <v>400</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23">
-        <v>56000023</v>
+        <v>56000121</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>166</v>
-      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L23" s="13">
+        <v>200</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="K23" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="L23" s="13">
-        <v>600</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>56000101</v>
+        <v>56000131</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>171</v>
-      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="14">
         <v>0</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="L24" s="13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
-        <v>56000102</v>
+        <v>56000201</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="14">
         <v>0</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="L25" s="13">
-        <v>800</v>
+        <v>163</v>
+      </c>
+      <c r="K25" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="L25" s="16">
+        <v>0</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26">
-        <v>56000111</v>
+      <c r="A26" s="11">
+        <v>56000202</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="34">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36">
         <v>102</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="I26" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="K26" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="L26" s="16">
         <v>0</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="14">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="L26" s="13">
-        <v>400</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27">
-        <v>56000121</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="14">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="L27" s="13">
-        <v>200</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28">
-        <v>56000131</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="14">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="L28" s="13">
-        <v>200</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29">
-        <v>56000201</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="14">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="K29" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="L29" s="16">
-        <v>0</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="11">
-        <v>56000202</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="D30" s="36">
-        <v>0</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38">
-        <v>102</v>
-      </c>
-      <c r="I30" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="J30" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="K30" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
-      <c r="M30" s="36" t="s">
-        <v>186</v>
+      <c r="M26" s="34" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3678,119 +3458,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
-        <v>128</v>
-      </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
         <v>124</v>
       </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
         <v>125</v>
       </c>
-      <c r="B6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" t="s">
-        <v>137</v>
-      </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix all the buff data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="176">
   <si>
     <t>stop</t>
   </si>
@@ -165,12 +165,6 @@
     <t>curse</t>
   </si>
   <si>
-    <t>感染</t>
-  </si>
-  <si>
-    <t>infect</t>
-  </si>
-  <si>
     <t>石化</t>
   </si>
   <si>
@@ -248,116 +242,304 @@
     <t>pa</t>
   </si>
   <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>ta</t>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除时</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnRemove</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高20%攻击和20%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnRound</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormatStringDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetDescript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuffEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Hp*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuffEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mark</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>静止</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>na</t>
-  </si>
-  <si>
-    <t>ns</t>
-  </si>
-  <si>
-    <t>ta</t>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>移除时</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnRemove</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高20%攻击和20%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低50%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低40%命中</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低25%命中和回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低30%速度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnRound</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少10%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FormatStringDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetDescript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuffEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Hp*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击，无法使用技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;103</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuffEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法被治疗，每回合减少5%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>atkr1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitr1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-100%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-80%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>全属性-60%</t>
+  </si>
+  <si>
+    <t>全属性-40%</t>
+  </si>
+  <si>
+    <t>全属性-20%</t>
+  </si>
+  <si>
+    <t>5回</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4回</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3回</t>
+  </si>
+  <si>
+    <t>2回</t>
+  </si>
+  <si>
+    <t>1回</t>
+  </si>
+  <si>
+    <t>1600分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200分</t>
+  </si>
+  <si>
+    <t>800分</t>
+  </si>
+  <si>
+    <t>400分</t>
+  </si>
+  <si>
+    <t>1600分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1280分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>960分</t>
+  </si>
+  <si>
+    <t>640分</t>
+  </si>
+  <si>
+    <t>320分</t>
+  </si>
+  <si>
+    <t>720分</t>
+  </si>
+  <si>
+    <t>480分</t>
+  </si>
+  <si>
+    <t>240分</t>
+  </si>
+  <si>
+    <t>160分</t>
+  </si>
+  <si>
+    <t>80分</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>色彩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,255,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>156,0,24</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>128,0,128</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,100,100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>196,196,196</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52,52,52</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,255,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,102,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>239,125,141</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,255,204</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,255,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,102,255</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>129,255,129</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>免疫组</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -365,317 +547,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Mark</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Hp*0.05);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>静止</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法被治疗，攻击时有20%几率击中自身</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少30%防御的生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Atk*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合减少30%攻击的生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低20%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高10%攻击和10%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防+2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高20%攻击和20%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻防-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>na</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低10%攻击和10%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>命避+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高10%命中和10%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>降低10%命中和10%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>命避-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>atkr1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hitr1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-100%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2000分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-80%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>全属性-60%</t>
-  </si>
-  <si>
-    <t>全属性-40%</t>
-  </si>
-  <si>
-    <t>全属性-20%</t>
-  </si>
-  <si>
-    <t>5回</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>4回</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3回</t>
-  </si>
-  <si>
-    <t>2回</t>
-  </si>
-  <si>
-    <t>1回</t>
-  </si>
-  <si>
-    <t>1600分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1200分</t>
-  </si>
-  <si>
-    <t>800分</t>
-  </si>
-  <si>
-    <t>400分</t>
-  </si>
-  <si>
-    <t>1600分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1280分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>960分</t>
-  </si>
-  <si>
-    <t>640分</t>
-  </si>
-  <si>
-    <t>320分</t>
-  </si>
-  <si>
-    <t>720分</t>
-  </si>
-  <si>
-    <t>480分</t>
-  </si>
-  <si>
-    <t>240分</t>
-  </si>
-  <si>
-    <t>160分</t>
-  </si>
-  <si>
-    <t>80分</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>色彩</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,0,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,255,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,0,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>156,0,24</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>128,0,128</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>100,100,100</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>196,196,196</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52,52,52</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,255,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,102,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>239,125,141</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,0,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,255,204</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,255,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,102,255</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>129,255,129</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击和使用技能，但会提高50%防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无法攻击和使用技能，但受到攻击后状态解除</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>免疫组</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Group</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -712,15 +583,167 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>216,114,30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>shield</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>EndOnHit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Spd-=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Spd+=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>速度-6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Def-=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Def+=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit-=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit+=6;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御-6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中-6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit-=5;o.Dhit-=5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit+=5;o.Dhit+=5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中-5，回避-5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>255,153,0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击有25%几率击中自身</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低25%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.25;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.25;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击和移动</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Atk*0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少当前生命的20%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少最大生命的10%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击、移动、使用技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击、移动、使用技能，但受到攻击后状态解除</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Def+=10;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Def-=10;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法攻击、移动、使用技能，但会提高10点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少攻击*0.5的生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.1;o.Def-=2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.2;o.Def+=4;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk/=0.2;o.Def-=4;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高10%攻击和2点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高20%攻击和4点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Atk*=0.1;o.Def+=2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低10%攻击和2点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit+=2;o.Dhit+=2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Hit-=2;o.Dhit-=2;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高2点命中和2点回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低2点命中和2点回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Hp*0.2);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1248,7 +1271,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD8721E"/>
+        <fgColor rgb="FFFF9900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2119,6 +2142,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FFD8721E"/>
       <color rgb="FFC10741"/>
       <color rgb="FF81FF81"/>
@@ -2128,7 +2152,6 @@
       <color rgb="FF00FFCC"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFEF7D8D"/>
-      <color rgb="FF006600"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2143,8 +2166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A3:M26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:M25"/>
   <sortState ref="A4:M30">
     <sortCondition ref="A3:A30"/>
   </sortState>
@@ -2454,13 +2477,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2477,125 +2500,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="K1" s="8" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2603,10 +2626,10 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -2618,16 +2641,16 @@
         <v>6</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="L4" s="13">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>0</v>
@@ -2641,28 +2664,32 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>138</v>
+      </c>
       <c r="G5" s="15"/>
       <c r="H5" s="14">
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="L5" s="13">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>2</v>
@@ -2676,28 +2703,32 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="14">
         <v>0</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="L6" s="13">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>4</v>
@@ -2711,32 +2742,32 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="L7" s="13">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>6</v>
@@ -2750,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -2758,20 +2789,20 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="14" t="s">
-        <v>72</v>
+      <c r="H8" s="14">
+        <v>103</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="L8" s="13">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>8</v>
@@ -2785,7 +2816,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -2793,22 +2824,22 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H9" s="14">
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="L9" s="13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>10</v>
@@ -2822,7 +2853,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4">
         <v>4</v>
@@ -2834,13 +2865,13 @@
         <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>69</v>
+        <v>154</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="L10" s="13">
         <v>2000</v>
@@ -2857,7 +2888,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -2865,19 +2896,19 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H11" s="14">
         <v>0</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="L11" s="13">
         <v>200</v>
@@ -2894,28 +2925,32 @@
         <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4">
         <v>3</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="G12" s="15"/>
       <c r="H12" s="14">
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="L12" s="13">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>16</v>
@@ -2929,7 +2964,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4">
         <v>3</v>
@@ -2938,16 +2973,16 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="L13" s="13">
         <v>2500</v>
@@ -2964,7 +2999,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -2972,22 +3007,22 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="H14" s="14">
         <v>0</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="L14" s="13">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>20</v>
@@ -3001,28 +3036,32 @@
         <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>147</v>
+      </c>
       <c r="G15" s="15"/>
       <c r="H15" s="14">
         <v>0</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>60</v>
+        <v>148</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="L15" s="13">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>22</v>
@@ -3030,36 +3069,38 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
-        <v>56000015</v>
+        <v>56000018</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" s="14">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>132</v>
+        <v>162</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L16" s="13">
-        <v>250</v>
+        <v>1500</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>24</v>
@@ -3067,31 +3108,31 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
-        <v>56000018</v>
+        <v>56000019</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="K17" s="23" t="s">
-        <v>137</v>
+        <v>48</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>120</v>
       </c>
       <c r="L17" s="13">
         <v>1500</v>
@@ -3102,34 +3143,38 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
-        <v>56000019</v>
+        <v>56000023</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>123</v>
+      </c>
       <c r="G18" s="15"/>
-      <c r="H18" s="14" t="s">
-        <v>70</v>
+      <c r="H18" s="14">
+        <v>101</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>145</v>
+        <v>49</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>121</v>
       </c>
       <c r="L18" s="13">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>28</v>
@@ -3137,204 +3182,208 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <v>56000023</v>
+        <v>56000101</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="14">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="31" t="s">
-        <v>146</v>
+        <v>167</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L19" s="13">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <v>56000101</v>
+        <v>56000102</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="14">
         <v>0</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="L20" s="13">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
-        <v>56000102</v>
+        <v>56000111</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="14">
         <v>0</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="L21" s="13">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
-        <v>56000111</v>
+        <v>56000121</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="D22" s="4">
         <v>0</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="14">
         <v>0</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="L22" s="13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23">
-        <v>56000121</v>
+        <v>56000131</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>171</v>
+      </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
         <v>0</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>95</v>
+        <v>174</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="L23" s="13">
         <v>200</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>56000131</v>
+        <v>56000201</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
@@ -3346,89 +3395,54 @@
         <v>0</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="L24" s="13">
-        <v>200</v>
+        <v>130</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="16">
+        <v>0</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25">
-        <v>56000201</v>
+      <c r="A25" s="11">
+        <v>56000202</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D25" s="4">
+        <v>133</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="34">
         <v>0</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="14">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>164</v>
+      <c r="G25" s="35"/>
+      <c r="H25" s="36">
+        <v>102</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" s="38" t="s">
+        <v>149</v>
       </c>
       <c r="L25" s="16">
         <v>0</v>
       </c>
-      <c r="M25" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="11">
-        <v>56000202</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="34">
-        <v>0</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36">
-        <v>102</v>
-      </c>
-      <c r="I26" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="K26" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="L26" s="16">
-        <v>0</v>
-      </c>
-      <c r="M26" s="34" t="s">
-        <v>169</v>
+      <c r="M25" s="34" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3458,119 +3472,119 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
element buff skill fin
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1729,6 +1729,18 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1744,18 +1756,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2183,8 +2183,8 @@
     <tableColumn id="9" name="EndOnHit" dataDxfId="4"/>
     <tableColumn id="11" name="GetDescript" dataDxfId="3"/>
     <tableColumn id="6" name="Color" dataDxfId="2"/>
-    <tableColumn id="4" name="Mark" dataDxfId="1"/>
-    <tableColumn id="13" name="Icon" dataDxfId="0"/>
+    <tableColumn id="4" name="Mark" dataDxfId="0"/>
+    <tableColumn id="13" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2483,7 +2483,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2495,7 +2495,7 @@
     <col min="10" max="10" width="34.75" customWidth="1"/>
     <col min="11" max="11" width="12.75" customWidth="1"/>
     <col min="12" max="12" width="6.125" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2650,7 +2650,7 @@
         <v>115</v>
       </c>
       <c r="L4" s="13">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>0</v>
@@ -2689,7 +2689,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="13">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>2</v>
@@ -2728,7 +2728,7 @@
         <v>113</v>
       </c>
       <c r="L6" s="13">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>4</v>
@@ -2767,7 +2767,7 @@
         <v>116</v>
       </c>
       <c r="L7" s="13">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>6</v>
@@ -2802,7 +2802,7 @@
         <v>118</v>
       </c>
       <c r="L8" s="13">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>8</v>
@@ -2839,7 +2839,7 @@
         <v>107</v>
       </c>
       <c r="L9" s="13">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>10</v>
@@ -2874,7 +2874,7 @@
         <v>108</v>
       </c>
       <c r="L10" s="13">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>12</v>
@@ -2911,7 +2911,7 @@
         <v>106</v>
       </c>
       <c r="L11" s="13">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>14</v>
@@ -2950,7 +2950,7 @@
         <v>111</v>
       </c>
       <c r="L12" s="13">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>16</v>
@@ -2985,7 +2985,7 @@
         <v>117</v>
       </c>
       <c r="L13" s="13">
-        <v>2500</v>
+        <v>125</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>18</v>
@@ -3022,7 +3022,7 @@
         <v>109</v>
       </c>
       <c r="L14" s="13">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>20</v>
@@ -3061,7 +3061,7 @@
         <v>110</v>
       </c>
       <c r="L15" s="13">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>22</v>
@@ -3100,7 +3100,7 @@
         <v>112</v>
       </c>
       <c r="L16" s="13">
-        <v>1500</v>
+        <v>75</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>24</v>
@@ -3135,7 +3135,7 @@
         <v>120</v>
       </c>
       <c r="L17" s="13">
-        <v>1500</v>
+        <v>75</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>26</v>
@@ -3174,7 +3174,7 @@
         <v>121</v>
       </c>
       <c r="L18" s="13">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>28</v>
@@ -3213,7 +3213,7 @@
         <v>119</v>
       </c>
       <c r="L19" s="13">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>73</v>
@@ -3252,7 +3252,7 @@
         <v>119</v>
       </c>
       <c r="L20" s="13">
-        <v>800</v>
+        <v>40</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>74</v>
@@ -3291,7 +3291,7 @@
         <v>119</v>
       </c>
       <c r="L21" s="13">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>75</v>
@@ -3330,7 +3330,7 @@
         <v>119</v>
       </c>
       <c r="L22" s="13">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>76</v>
@@ -3369,7 +3369,7 @@
         <v>119</v>
       </c>
       <c r="L23" s="13">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
#8 finish terrain monster card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="177">
   <si>
     <t>stop</t>
   </si>
@@ -744,6 +744,10 @@
   </si>
   <si>
     <t>o.AddHp(-o.Hp*0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>56000023|Tile</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1729,18 +1733,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1756,6 +1748,18 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2183,8 +2187,8 @@
     <tableColumn id="9" name="EndOnHit" dataDxfId="4"/>
     <tableColumn id="11" name="GetDescript" dataDxfId="3"/>
     <tableColumn id="6" name="Color" dataDxfId="2"/>
-    <tableColumn id="4" name="Mark" dataDxfId="0"/>
-    <tableColumn id="13" name="Icon" dataDxfId="1"/>
+    <tableColumn id="4" name="Mark" dataDxfId="1"/>
+    <tableColumn id="13" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2480,22 +2484,22 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="3" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="7" width="15.625" customWidth="1"/>
-    <col min="9" max="9" width="6.375" customWidth="1"/>
-    <col min="10" max="10" width="34.75" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="6.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="3" max="4" width="6.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="34.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2808,7 +2812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="21.6">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2880,7 +2884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="21.6">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -2991,7 +2995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="21.6">
       <c r="A14">
         <v>56000013</v>
       </c>
@@ -3028,7 +3032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="21.6">
       <c r="A15">
         <v>56000014</v>
       </c>
@@ -3142,8 +3146,8 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18">
-        <v>56000023</v>
+      <c r="A18" t="s">
+        <v>176</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>27</v>
@@ -3180,7 +3184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="21.6">
       <c r="A19">
         <v>56000101</v>
       </c>
@@ -3219,7 +3223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" ht="21.6">
       <c r="A20">
         <v>56000102</v>
       </c>
@@ -3258,7 +3262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" ht="21.6">
       <c r="A21">
         <v>56000111</v>
       </c>
@@ -3297,7 +3301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="21.6">
       <c r="A22">
         <v>56000121</v>
       </c>
@@ -3336,7 +3340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" ht="21.6">
       <c r="A23">
         <v>56000131</v>
       </c>
@@ -3464,10 +3468,10 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="6" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="6" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
finish the stop auro
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -2484,10 +2484,10 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
fix some spell card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -2487,19 +2487,19 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="3" max="4" width="6.77734375" customWidth="1"/>
-    <col min="5" max="7" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="34.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="3" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="7" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="6.375" customWidth="1"/>
+    <col min="10" max="10" width="34.75" customWidth="1"/>
+    <col min="11" max="11" width="12.75" customWidth="1"/>
+    <col min="12" max="12" width="6.125" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2812,7 +2812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21.6">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21.6">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21.6">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>56000013</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21.6">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>56000014</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21.6">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>56000101</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21.6">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>56000102</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21.6">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>56000111</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21.6">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>56000121</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21.6">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>56000131</v>
       </c>
@@ -3468,10 +3468,10 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="6" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
close #52 saint shield now is a parmor skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -2487,19 +2487,19 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="3" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="7" width="15.625" customWidth="1"/>
-    <col min="9" max="9" width="6.375" customWidth="1"/>
-    <col min="10" max="10" width="34.75" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="6.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="3" max="4" width="6.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="34.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2812,7 +2812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="21.6">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="21.6">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="21.6">
       <c r="A14">
         <v>56000013</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="21.6">
       <c r="A15">
         <v>56000014</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="21.6">
       <c r="A19">
         <v>56000101</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" ht="21.6">
       <c r="A20">
         <v>56000102</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" ht="21.6">
       <c r="A21">
         <v>56000111</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="21.6">
       <c r="A22">
         <v>56000121</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" ht="21.6">
       <c r="A23">
         <v>56000131</v>
       </c>
@@ -3468,10 +3468,10 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="6" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="6" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
support multi MagicRegions, e.g. one for spell, one for attack range
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -511,10 +511,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0,0,0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0,255,204</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -748,14 +744,18 @@
   </si>
   <si>
     <t>56000023|Tile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>30,30,50</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,12 +1245,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1276,6 +1270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1E1E32"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1653,19 +1653,16 @@
     <xf numFmtId="49" fontId="0" fillId="46" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="50" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
@@ -1683,7 +1680,10 @@
     <xf numFmtId="49" fontId="26" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2146,6 +2146,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1E1E32"/>
       <color rgb="FFFF9900"/>
       <color rgb="FFD8721E"/>
       <color rgb="FFC10741"/>
@@ -2155,7 +2156,6 @@
       <color rgb="FFFF6600"/>
       <color rgb="FF00FFCC"/>
       <color rgb="FFFF0000"/>
-      <color rgb="FFEF7D8D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2195,7 +2195,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2270,6 +2270,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2305,6 +2322,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2487,22 +2521,22 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="3" max="4" width="6.77734375" customWidth="1"/>
-    <col min="5" max="7" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="34.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="3" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="7" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="6.375" customWidth="1"/>
+    <col min="10" max="10" width="34.75" customWidth="1"/>
+    <col min="11" max="11" width="12.75" customWidth="1"/>
+    <col min="12" max="12" width="6.125" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -2513,7 +2547,7 @@
         <v>33</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>51</v>
@@ -2543,7 +2577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -2554,7 +2588,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>62</v>
@@ -2584,7 +2618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
@@ -2595,7 +2629,7 @@
         <v>39</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>50</v>
@@ -2610,7 +2644,7 @@
         <v>40</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>58</v>
@@ -2625,7 +2659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>56000001</v>
       </c>
@@ -2648,7 +2682,7 @@
         <v>49</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K4" s="26" t="s">
         <v>115</v>
@@ -2660,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>56000002</v>
       </c>
@@ -2674,10 +2708,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>138</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="14">
@@ -2687,7 +2721,7 @@
         <v>49</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>114</v>
@@ -2699,7 +2733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>56000003</v>
       </c>
@@ -2713,10 +2747,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>140</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>141</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="14">
@@ -2726,7 +2760,7 @@
         <v>49</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" s="24" t="s">
         <v>113</v>
@@ -2738,7 +2772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>56000004</v>
       </c>
@@ -2752,10 +2786,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
@@ -2765,7 +2799,7 @@
         <v>49</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="27" t="s">
         <v>116</v>
@@ -2777,7 +2811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>56000006</v>
       </c>
@@ -2800,10 +2834,10 @@
         <v>49</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>118</v>
+        <v>149</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>117</v>
       </c>
       <c r="L8" s="13">
         <v>50</v>
@@ -2812,7 +2846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21.6">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2837,7 +2871,7 @@
         <v>49</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>107</v>
@@ -2849,7 +2883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>56000009</v>
       </c>
@@ -2872,7 +2906,7 @@
         <v>49</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>108</v>
@@ -2884,7 +2918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21.6">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -2900,7 +2934,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H11" s="14">
         <v>0</v>
@@ -2909,7 +2943,7 @@
         <v>49</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>106</v>
@@ -2921,7 +2955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>56000011</v>
       </c>
@@ -2935,10 +2969,10 @@
         <v>3</v>
       </c>
       <c r="E12" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>143</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="14">
@@ -2948,7 +2982,7 @@
         <v>49</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K12" s="22" t="s">
         <v>111</v>
@@ -2960,7 +2994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>56000012</v>
       </c>
@@ -2983,10 +3017,10 @@
         <v>49</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>117</v>
+        <v>157</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>176</v>
       </c>
       <c r="L13" s="13">
         <v>125</v>
@@ -2995,7 +3029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21.6">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>56000013</v>
       </c>
@@ -3011,7 +3045,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H14" s="14">
         <v>0</v>
@@ -3020,7 +3054,7 @@
         <v>49</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>109</v>
@@ -3032,7 +3066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21.6">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>56000014</v>
       </c>
@@ -3046,10 +3080,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="14">
@@ -3059,7 +3093,7 @@
         <v>49</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>110</v>
@@ -3071,7 +3105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>56000018</v>
       </c>
@@ -3085,10 +3119,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>161</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="14" t="s">
@@ -3098,7 +3132,7 @@
         <v>49</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K16" s="23" t="s">
         <v>112</v>
@@ -3110,7 +3144,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>56000019</v>
       </c>
@@ -3133,10 +3167,10 @@
         <v>48</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>120</v>
+        <v>158</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="L17" s="13">
         <v>40</v>
@@ -3145,9 +3179,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>27</v>
@@ -3159,10 +3193,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="14">
@@ -3174,8 +3208,8 @@
       <c r="J18" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="31" t="s">
-        <v>121</v>
+      <c r="K18" s="30" t="s">
+        <v>120</v>
       </c>
       <c r="L18" s="13">
         <v>30</v>
@@ -3184,7 +3218,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21.6">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>56000101</v>
       </c>
@@ -3198,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="14">
@@ -3211,10 +3245,10 @@
         <v>49</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L19" s="13">
         <v>20</v>
@@ -3223,7 +3257,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21.6">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>56000102</v>
       </c>
@@ -3237,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="14">
@@ -3250,10 +3284,10 @@
         <v>49</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L20" s="13">
         <v>40</v>
@@ -3262,7 +3296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21.6">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>56000111</v>
       </c>
@@ -3276,10 +3310,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="14">
@@ -3289,10 +3323,10 @@
         <v>49</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L21" s="13">
         <v>20</v>
@@ -3301,7 +3335,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21.6">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>56000121</v>
       </c>
@@ -3315,10 +3349,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>171</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="14">
@@ -3328,10 +3362,10 @@
         <v>49</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L22" s="13">
         <v>10</v>
@@ -3340,7 +3374,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21.6">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>56000131</v>
       </c>
@@ -3354,10 +3388,10 @@
         <v>0</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
@@ -3367,10 +3401,10 @@
         <v>49</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L23" s="13">
         <v>10</v>
@@ -3379,15 +3413,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>56000201</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
@@ -3402,51 +3436,51 @@
         <v>49</v>
       </c>
       <c r="J24" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" s="31" t="s">
         <v>130</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>131</v>
       </c>
       <c r="L24" s="16">
         <v>0</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="11">
         <v>56000202</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="34">
+        <v>132</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="33">
         <v>0</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36">
+      <c r="G25" s="34"/>
+      <c r="H25" s="35">
         <v>102</v>
       </c>
-      <c r="I25" s="37" t="s">
+      <c r="I25" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="K25" s="38" t="s">
-        <v>149</v>
+      <c r="J25" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="K25" s="37" t="s">
+        <v>148</v>
       </c>
       <c r="L25" s="16">
         <v>0</v>
       </c>
-      <c r="M25" s="34" t="s">
-        <v>135</v>
+      <c r="M25" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3468,13 +3502,14 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="6" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>78</v>
       </c>
@@ -3491,7 +3526,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -3511,7 +3546,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3531,7 +3566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -3551,7 +3586,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -3571,7 +3606,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
fix a bug of some monster skill not effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -300,10 +300,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.Hp*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>2;5</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -659,10 +655,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.Atk*0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>每回合减少当前生命的20%</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -748,6 +740,14 @@
   </si>
   <si>
     <t>30,30,50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.MaxHp.Source*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Atk.Source*0.5);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2521,7 +2521,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2547,7 +2547,7 @@
         <v>33</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>51</v>
@@ -2568,10 +2568,10 @@
         <v>36</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>43</v>
@@ -2588,10 +2588,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>59</v>
@@ -2609,10 +2609,10 @@
         <v>57</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>30</v>
@@ -2629,7 +2629,7 @@
         <v>39</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>50</v>
@@ -2644,16 +2644,16 @@
         <v>40</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>42</v>
@@ -2664,7 +2664,7 @@
         <v>56000001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>45</v>
@@ -2682,10 +2682,10 @@
         <v>49</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L4" s="13">
         <v>25</v>
@@ -2708,10 +2708,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="14">
@@ -2721,10 +2721,10 @@
         <v>49</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L5" s="13">
         <v>30</v>
@@ -2747,10 +2747,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="14">
@@ -2760,10 +2760,10 @@
         <v>49</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="13">
         <v>30</v>
@@ -2786,10 +2786,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="14">
@@ -2799,10 +2799,10 @@
         <v>49</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L7" s="13">
         <v>25</v>
@@ -2834,10 +2834,10 @@
         <v>49</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L8" s="13">
         <v>50</v>
@@ -2846,7 +2846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2862,7 +2862,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="H9" s="14">
         <v>0</v>
@@ -2871,10 +2871,10 @@
         <v>49</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L9" s="13">
         <v>20</v>
@@ -2906,10 +2906,10 @@
         <v>49</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L10" s="13">
         <v>50</v>
@@ -2918,7 +2918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="H11" s="14">
         <v>0</v>
@@ -2943,10 +2943,10 @@
         <v>49</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L11" s="13">
         <v>10</v>
@@ -2969,10 +2969,10 @@
         <v>3</v>
       </c>
       <c r="E12" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>141</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>142</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="14">
@@ -2982,10 +2982,10 @@
         <v>49</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L12" s="13">
         <v>30</v>
@@ -3011,16 +3011,16 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K13" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L13" s="13">
         <v>125</v>
@@ -3045,7 +3045,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H14" s="14">
         <v>0</v>
@@ -3054,10 +3054,10 @@
         <v>49</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L14" s="13">
         <v>25</v>
@@ -3080,10 +3080,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>146</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="14">
@@ -3093,10 +3093,10 @@
         <v>49</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L15" s="13">
         <v>50</v>
@@ -3119,23 +3119,23 @@
         <v>4</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L16" s="13">
         <v>40</v>
@@ -3161,16 +3161,16 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L17" s="13">
         <v>40</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>27</v>
@@ -3193,10 +3193,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="14">
@@ -3209,7 +3209,7 @@
         <v>54</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L18" s="13">
         <v>30</v>
@@ -3223,7 +3223,7 @@
         <v>56000101</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>44</v>
@@ -3232,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="14">
@@ -3245,16 +3245,16 @@
         <v>49</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L19" s="13">
         <v>20</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
@@ -3262,7 +3262,7 @@
         <v>56000102</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>44</v>
@@ -3271,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="14">
@@ -3284,16 +3284,16 @@
         <v>49</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L20" s="13">
         <v>40</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.15">
@@ -3301,19 +3301,19 @@
         <v>56000111</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="14">
@@ -3323,16 +3323,16 @@
         <v>49</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L21" s="13">
         <v>20</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
@@ -3340,7 +3340,7 @@
         <v>56000121</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>44</v>
@@ -3349,10 +3349,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="14">
@@ -3362,16 +3362,16 @@
         <v>49</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L22" s="13">
         <v>10</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
@@ -3379,19 +3379,19 @@
         <v>56000131</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="14">
@@ -3401,16 +3401,16 @@
         <v>49</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L23" s="13">
         <v>10</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
@@ -3418,10 +3418,10 @@
         <v>56000201</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
@@ -3436,16 +3436,16 @@
         <v>49</v>
       </c>
       <c r="J24" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="K24" s="31" t="s">
         <v>129</v>
-      </c>
-      <c r="K24" s="31" t="s">
-        <v>130</v>
       </c>
       <c r="L24" s="16">
         <v>0</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.15">
@@ -3453,10 +3453,10 @@
         <v>56000202</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="33">
         <v>0</v>
@@ -3471,16 +3471,16 @@
         <v>48</v>
       </c>
       <c r="J25" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K25" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L25" s="16">
         <v>0</v>
       </c>
       <c r="M25" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3511,119 +3511,119 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>99</v>
-      </c>
-      <c r="F4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
         <v>96</v>
       </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>101</v>
-      </c>
-      <c r="F6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new excel alias name load method
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\Tool\ExcelToCsv\bin\Debug\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="180">
   <si>
     <t>stop</t>
   </si>
@@ -735,10 +735,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>56000023|Tile</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>30,30,50</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -748,6 +744,22 @@
   </si>
   <si>
     <t>o.AddHp(-o.Atk.Source*0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>别名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tile</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1590,15 +1602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1685,6 +1688,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2145,6 +2157,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF1E1E32"/>
       <color rgb="FFFF9900"/>
@@ -2170,13 +2248,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:M25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A3:M25"/>
-  <sortState ref="A4:M30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:N25"/>
+  <sortState ref="A4:N30">
     <sortCondition ref="A3:A30"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="14">
     <tableColumn id="1" name="Id" dataDxfId="12"/>
+    <tableColumn id="7" name="Alias"/>
     <tableColumn id="2" name="Name" dataDxfId="11"/>
     <tableColumn id="3" name="Type" dataDxfId="10"/>
     <tableColumn id="5" name="Group" dataDxfId="9"/>
@@ -2202,7 +2281,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2515,971 +2594,985 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="3" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="7" width="15.625" customWidth="1"/>
-    <col min="9" max="9" width="6.375" customWidth="1"/>
-    <col min="10" max="10" width="34.75" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="6.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="4" max="5" width="6.75" customWidth="1"/>
+    <col min="6" max="8" width="15.625" customWidth="1"/>
+    <col min="10" max="10" width="6.375" customWidth="1"/>
+    <col min="11" max="11" width="34.75" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="6.125" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>56000001</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="14">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="11">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="L4" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L4" s="13">
+      <c r="M4" s="10">
         <v>25</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>56000002</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="14">
+      <c r="H5" s="12"/>
+      <c r="I5" s="11">
         <v>0</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="L5" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="13">
+      <c r="M5" s="10">
         <v>30</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>56000003</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="14">
+      <c r="H6" s="12"/>
+      <c r="I6" s="11">
         <v>0</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="L6" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="L6" s="13">
+      <c r="M6" s="10">
         <v>30</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>56000004</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14">
+      <c r="H7" s="12"/>
+      <c r="I7" s="11">
         <v>0</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="K7" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="L7" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="L7" s="13">
+      <c r="M7" s="10">
         <v>25</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>56000006</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="14">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="11">
         <v>103</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="K8" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="L8" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="L8" s="13">
+      <c r="M8" s="10">
         <v>50</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>56000007</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="13">
+      <c r="M9" s="10">
         <v>20</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>56000009</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="11">
         <v>2</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="L10" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="L10" s="13">
+      <c r="M10" s="10">
         <v>50</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="22.5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>56000010</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>4</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="14">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="K11" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="L11" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="13">
+      <c r="M11" s="10">
         <v>10</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>56000011</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>3</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="F12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="G12" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="14">
+      <c r="H12" s="12"/>
+      <c r="I12" s="11">
         <v>0</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="K12" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="L12" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="L12" s="13">
+      <c r="M12" s="10">
         <v>30</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>56000012</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K13" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="L13" s="13">
+      <c r="L13" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="M13" s="10">
         <v>125</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>56000013</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="H14" s="14">
+      <c r="I14" s="11">
         <v>0</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="K14" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="L14" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="L14" s="13">
+      <c r="M14" s="10">
         <v>25</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>56000014</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14">
+      <c r="H15" s="12"/>
+      <c r="I15" s="11">
         <v>0</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="K15" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="L15" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="L15" s="13">
+      <c r="M15" s="10">
         <v>50</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>56000018</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>4</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="F16" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="G16" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="K16" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="L16" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L16" s="13">
+      <c r="M16" s="10">
         <v>40</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>56000019</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="L17" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="L17" s="13">
+      <c r="M17" s="10">
         <v>40</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="N17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>56000023</v>
+      </c>
+      <c r="B18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="F18" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="G18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14">
+      <c r="H18" s="12"/>
+      <c r="I18" s="11">
         <v>101</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="K18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="L18" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="L18" s="13">
+      <c r="M18" s="10">
         <v>30</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="N18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>56000101</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="F19" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="G19" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14">
+      <c r="H19" s="12"/>
+      <c r="I19" s="11">
         <v>0</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="K19" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L19" s="13">
+      <c r="M19" s="10">
         <v>20</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>56000102</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="F20" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="G20" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14">
+      <c r="H20" s="12"/>
+      <c r="I20" s="11">
         <v>0</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="K20" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="13">
+      <c r="M20" s="10">
         <v>40</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="N20" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>56000111</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="4">
+      <c r="E21" s="4">
         <v>0</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="G21" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="14">
+      <c r="H21" s="12"/>
+      <c r="I21" s="11">
         <v>0</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="K21" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L21" s="13">
+      <c r="M21" s="10">
         <v>20</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="N21" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>56000121</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="4">
+      <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="F22" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="G22" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="14">
+      <c r="H22" s="12"/>
+      <c r="I22" s="11">
         <v>0</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="K22" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L22" s="13">
+      <c r="M22" s="10">
         <v>10</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="N22" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>56000131</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="4">
+      <c r="E23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="F23" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="G23" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="14">
+      <c r="H23" s="12"/>
+      <c r="I23" s="11">
         <v>0</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="K23" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L23" s="13">
+      <c r="M23" s="10">
         <v>10</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>56000201</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E24" s="4">
         <v>0</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="14">
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="11">
         <v>0</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="K24" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="L24" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="L24" s="16">
+      <c r="M24" s="13">
         <v>0</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="N24" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A25" s="11">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A25" s="8">
         <v>56000202</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="D25" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="33">
+      <c r="E25" s="30">
         <v>0</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35">
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="32">
         <v>102</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="J25" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="K25" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="K25" s="37" t="s">
+      <c r="L25" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="L25" s="16">
+      <c r="M25" s="13">
         <v>0</v>
       </c>
-      <c r="M25" s="33" t="s">
+      <c r="N25" s="30" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add some bird and fish cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\Tool\ExcelToCsv\bin\Debug\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -659,10 +659,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每回合减少最大生命的10%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法攻击、移动、使用技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -683,10 +679,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每回合减少攻击*0.5的生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>o.Atk/=0.1;o.Def-=2;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -739,14 +731,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.MaxHp.Source*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.AddHp(-o.Atk.Source*0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>别名</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -760,6 +744,22 @@
   </si>
   <si>
     <t>Tile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少最大生命的15%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.MaxHp.Source*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合减少攻击*0.8的生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Atk.Source*0.8);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2157,72 +2157,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FF1E1E32"/>
       <color rgb="FFFF9900"/>
@@ -2281,7 +2215,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2600,7 +2534,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2621,7 +2555,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>32</v>
@@ -2665,7 +2599,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
@@ -2709,7 +2643,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -2935,7 +2869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>56000007</v>
       </c>
@@ -2951,7 +2885,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -2960,7 +2894,7 @@
         <v>49</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>106</v>
@@ -3023,7 +2957,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I11" s="11">
         <v>0</v>
@@ -3032,13 +2966,13 @@
         <v>49</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>105</v>
       </c>
       <c r="M11" s="10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>14</v>
@@ -3106,10 +3040,10 @@
         <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M13" s="10">
         <v>125</v>
@@ -3134,7 +3068,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I14" s="11">
         <v>0</v>
@@ -3208,10 +3142,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>158</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="11" t="s">
@@ -3221,7 +3155,7 @@
         <v>49</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L16" s="20" t="s">
         <v>111</v>
@@ -3256,7 +3190,7 @@
         <v>48</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L17" s="26" t="s">
         <v>118</v>
@@ -3273,7 +3207,7 @@
         <v>56000023</v>
       </c>
       <c r="B18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>27</v>
@@ -3324,10 +3258,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="11">
@@ -3337,7 +3271,7 @@
         <v>49</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>117</v>
@@ -3363,10 +3297,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="11">
@@ -3376,7 +3310,7 @@
         <v>49</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>117</v>
@@ -3402,10 +3336,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="11">
@@ -3415,7 +3349,7 @@
         <v>49</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>117</v>
@@ -3441,10 +3375,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="11">
@@ -3454,7 +3388,7 @@
         <v>49</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>117</v>
@@ -3480,10 +3414,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="11">
@@ -3493,7 +3427,7 @@
         <v>49</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
optimise the resist of buffs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
           <t xml:space="preserve">
 1.生命
 2.意志
-3.肉体
+3.物理
 4.元素
 5.联动</t>
         </r>
@@ -2157,6 +2157,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF1E1E32"/>
       <color rgb="FFFF9900"/>
@@ -2215,7 +2281,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2534,7 +2600,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
remake the attr implement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Buff" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
   <si>
     <t>stop</t>
   </si>
@@ -276,10 +276,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>提高20%攻击和20%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>每回合</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -523,14 +519,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk*=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>免疫组</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -583,34 +571,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Spd-=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Spd+=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>速度-6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Def-=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Def+=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit-=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit+=6;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>防御-6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -619,14 +583,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Hit-=5;o.Dhit-=5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit+=5;o.Dhit+=5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>命中-5，回避-5</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -643,14 +599,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.25;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.25;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法攻击和移动</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -667,30 +615,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Def+=10;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Def-=10;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>无法攻击、移动、使用技能，但会提高10点防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk/=0.1;o.Def-=2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk*=0.2;o.Def+=4;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Atk/=0.2;o.Def-=4;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提高10%攻击和2点防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -699,22 +627,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Atk*=0.1;o.Def+=2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>降低10%攻击和2点防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Hit+=2;o.Dhit+=2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Hit-=2;o.Dhit-=2;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提高2点命中和2点回避</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -751,31 +667,79 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.MaxHp.Source*0.15);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>每回合减少攻击*0.8的生命</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.AddHp(-o.Atk.Source*0.8);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>速度+8</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>o.Spd-=8;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o.Spd+=8;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>风怒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Spd",-6);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Def",-6);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Hit",-6);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Hit",-5);o.Action.AddAttrModify("Buff",buf.Id,"Dhit",-5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Def",10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.MaxHp*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.AddHp(-o.Atk*0.8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Spd",8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Atk",-o.Atk*0.25);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Atk",o.Atk*0.2);o.Action.AddAttrModify("Buff",buf.Id,"Dhit",2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高20%攻击和2点回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Atk",o.Atk*0.1);o.Action.AddAttrModify("Buff",buf.Id,"Def",2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Atk",o.Atk*0.2);o.Action.AddAttrModify("Buff",buf.Id,"Def",4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Atk",-o.Atk*0.1);o.Action.AddAttrModify("Buff",buf.Id,"Def",-2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Hit",2);o.Action.AddAttrModify("Buff",buf.Id,"Dhit",2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>o.Action.AddAttrModify("Buff",buf.Id,"Hit",-2);o.Action.AddAttrModify("Buff",buf.Id,"Dhit",-2);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2622,10 +2586,10 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2647,7 +2611,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>32</v>
@@ -2656,7 +2620,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>51</v>
@@ -2665,7 +2629,7 @@
         <v>52</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>34</v>
@@ -2677,10 +2641,10 @@
         <v>36</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N1" s="38" t="s">
         <v>43</v>
@@ -2691,7 +2655,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
@@ -2700,16 +2664,16 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>41</v>
@@ -2718,13 +2682,13 @@
         <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>30</v>
@@ -2735,7 +2699,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -2744,7 +2708,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>50</v>
@@ -2753,22 +2717,22 @@
         <v>53</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>40</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>42</v>
@@ -2779,7 +2743,7 @@
         <v>56000001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>45</v>
@@ -2797,10 +2761,10 @@
         <v>49</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M4" s="10">
         <v>25</v>
@@ -2809,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>56000002</v>
       </c>
@@ -2823,11 +2787,9 @@
         <v>3</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>136</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="11">
         <v>0</v>
@@ -2836,10 +2798,10 @@
         <v>49</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M5" s="10">
         <v>30</v>
@@ -2848,7 +2810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>56000003</v>
       </c>
@@ -2862,11 +2824,9 @@
         <v>2</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>139</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="11">
         <v>0</v>
@@ -2875,10 +2835,10 @@
         <v>49</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M6" s="10">
         <v>30</v>
@@ -2887,7 +2847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>56000004</v>
       </c>
@@ -2901,11 +2861,9 @@
         <v>3</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>151</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="11">
         <v>0</v>
@@ -2914,10 +2872,10 @@
         <v>49</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M7" s="10">
         <v>25</v>
@@ -2949,10 +2907,10 @@
         <v>49</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M8" s="10">
         <v>50</v>
@@ -2977,7 +2935,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -2986,10 +2944,10 @@
         <v>49</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M9" s="10">
         <v>20</v>
@@ -3021,10 +2979,10 @@
         <v>49</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M10" s="10">
         <v>50</v>
@@ -3033,7 +2991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>56000010</v>
       </c>
@@ -3049,7 +3007,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="I11" s="11">
         <v>0</v>
@@ -3058,10 +3016,10 @@
         <v>49</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M11" s="10">
         <v>20</v>
@@ -3070,7 +3028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>56000011</v>
       </c>
@@ -3084,11 +3042,9 @@
         <v>3</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>141</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="11">
         <v>0</v>
@@ -3097,10 +3053,10 @@
         <v>49</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M12" s="10">
         <v>30</v>
@@ -3126,16 +3082,16 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="M13" s="10">
         <v>125</v>
@@ -3160,7 +3116,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="I14" s="11">
         <v>0</v>
@@ -3169,10 +3125,10 @@
         <v>49</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M14" s="10">
         <v>25</v>
@@ -3181,7 +3137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>56000014</v>
       </c>
@@ -3195,11 +3151,9 @@
         <v>2</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>145</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="11">
         <v>0</v>
@@ -3208,10 +3162,10 @@
         <v>49</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M15" s="10">
         <v>50</v>
@@ -3220,7 +3174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>56000018</v>
       </c>
@@ -3234,23 +3188,21 @@
         <v>4</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>157</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M16" s="10">
         <v>40</v>
@@ -3276,16 +3228,16 @@
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>48</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M17" s="10">
         <v>40</v>
@@ -3294,12 +3246,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>56000023</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>27</v>
@@ -3311,11 +3263,9 @@
         <v>0</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>121</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="11">
         <v>101</v>
@@ -3324,10 +3274,10 @@
         <v>49</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M18" s="10">
         <v>30</v>
@@ -3336,12 +3286,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" ht="56.25" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>56000101</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>44</v>
@@ -3350,11 +3300,9 @@
         <v>0</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>159</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="11">
         <v>0</v>
@@ -3363,24 +3311,24 @@
         <v>49</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M19" s="10">
         <v>20</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" ht="56.25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>56000102</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>44</v>
@@ -3389,11 +3337,9 @@
         <v>0</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>161</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="11">
         <v>0</v>
@@ -3402,37 +3348,35 @@
         <v>49</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M20" s="10">
         <v>40</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>56000111</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>164</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="11">
         <v>0</v>
@@ -3441,24 +3385,24 @@
         <v>49</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M21" s="10">
         <v>20</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" ht="56.25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>56000121</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>44</v>
@@ -3467,11 +3411,9 @@
         <v>0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>167</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="11">
         <v>0</v>
@@ -3480,37 +3422,35 @@
         <v>49</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M22" s="10">
         <v>10</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>56000131</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>166</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="11">
         <v>0</v>
@@ -3519,16 +3459,16 @@
         <v>49</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M23" s="10">
         <v>10</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -3537,10 +3477,10 @@
       </c>
       <c r="B24" s="39"/>
       <c r="C24" s="40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
@@ -3555,16 +3495,16 @@
         <v>49</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M24" s="13">
         <v>0</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
@@ -3573,10 +3513,10 @@
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E25" s="30">
         <v>0</v>
@@ -3591,38 +3531,36 @@
         <v>48</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L25" s="34" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="M25" s="13">
         <v>0</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
       <c r="A26" s="40">
         <v>56000203</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E26" s="30">
         <v>0</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>181</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="G26" s="12"/>
       <c r="H26" s="31"/>
       <c r="I26" s="32">
         <v>0</v>
@@ -3631,16 +3569,16 @@
         <v>48</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="L26" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M26" s="13">
         <v>30</v>
       </c>
       <c r="N26" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3671,119 +3609,119 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>81</v>
-      </c>
-      <c r="F1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
-      </c>
-      <c r="F2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>94</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>95</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>98</v>
-      </c>
-      <c r="F4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
         <v>95</v>
       </c>
-      <c r="D5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>99</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>100</v>
-      </c>
-      <c r="F6" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimise some code format
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="176">
   <si>
     <t>stop</t>
   </si>
@@ -740,6 +740,10 @@
   </si>
   <si>
     <t>o.Action.AddAttrModify("Buff",buf.Id,"Hit",-2);o.Action.AddAttrModify("Buff",buf.Id,"Dhit",-2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1560,7 +1564,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1682,9 +1686,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2589,7 +2590,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3577,8 +3578,8 @@
       <c r="M26" s="13">
         <v>30</v>
       </c>
-      <c r="N26" s="41" t="s">
-        <v>130</v>
+      <c r="N26" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a new holy stone
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
   <si>
     <t>stop</t>
   </si>
@@ -744,6 +744,10 @@
   </si>
   <si>
     <t>wind</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HolyShield</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2587,10 +2591,10 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3512,7 +3516,9 @@
       <c r="A25" s="40">
         <v>56000202</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="40" t="s">
+        <v>176</v>
+      </c>
       <c r="C25" s="40" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
remove weapon skill on weapon break up
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Buff.xlsx
+++ b/ConfigData/Xlsx/Buff.xlsx
@@ -336,14 +336,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>命避+1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>命避-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>atk1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -748,6 +740,14 @@
   </si>
   <si>
     <t>HolyShield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命避-2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2591,10 +2591,10 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2616,7 +2616,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>32</v>
@@ -2625,7 +2625,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>51</v>
@@ -2646,7 +2646,7 @@
         <v>36</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M1" s="37" t="s">
         <v>61</v>
@@ -2660,7 +2660,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
@@ -2669,7 +2669,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>60</v>
@@ -2690,7 +2690,7 @@
         <v>56</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>62</v>
@@ -2704,7 +2704,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -2713,7 +2713,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>50</v>
@@ -2728,13 +2728,13 @@
         <v>40</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>57</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>63</v>
@@ -2766,10 +2766,10 @@
         <v>49</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M4" s="10">
         <v>25</v>
@@ -2792,7 +2792,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -2803,10 +2803,10 @@
         <v>49</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M5" s="10">
         <v>30</v>
@@ -2829,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -2840,10 +2840,10 @@
         <v>49</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M6" s="10">
         <v>30</v>
@@ -2866,7 +2866,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -2877,10 +2877,10 @@
         <v>49</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M7" s="10">
         <v>25</v>
@@ -2912,10 +2912,10 @@
         <v>49</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M8" s="10">
         <v>50</v>
@@ -2940,7 +2940,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -2949,10 +2949,10 @@
         <v>49</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M9" s="10">
         <v>20</v>
@@ -2984,10 +2984,10 @@
         <v>49</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M10" s="10">
         <v>50</v>
@@ -3012,7 +3012,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I11" s="11">
         <v>0</v>
@@ -3021,10 +3021,10 @@
         <v>49</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M11" s="10">
         <v>20</v>
@@ -3047,7 +3047,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -3058,10 +3058,10 @@
         <v>49</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M12" s="10">
         <v>30</v>
@@ -3093,10 +3093,10 @@
         <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M13" s="10">
         <v>125</v>
@@ -3121,7 +3121,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I14" s="11">
         <v>0</v>
@@ -3130,10 +3130,10 @@
         <v>49</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M14" s="10">
         <v>25</v>
@@ -3156,7 +3156,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -3167,10 +3167,10 @@
         <v>49</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M15" s="10">
         <v>50</v>
@@ -3193,7 +3193,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -3204,10 +3204,10 @@
         <v>49</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M16" s="10">
         <v>40</v>
@@ -3239,10 +3239,10 @@
         <v>48</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M17" s="10">
         <v>40</v>
@@ -3256,7 +3256,7 @@
         <v>56000023</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>27</v>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
@@ -3279,10 +3279,10 @@
         <v>49</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M18" s="10">
         <v>30</v>
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -3316,16 +3316,16 @@
         <v>49</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M19" s="10">
         <v>20</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="56.25" x14ac:dyDescent="0.15">
@@ -3342,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -3353,16 +3353,16 @@
         <v>49</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M20" s="10">
         <v>40</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
@@ -3379,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -3390,16 +3390,16 @@
         <v>49</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M21" s="10">
         <v>20</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="56.25" x14ac:dyDescent="0.15">
@@ -3407,7 +3407,7 @@
         <v>56000121</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>44</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -3427,16 +3427,16 @@
         <v>49</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M22" s="10">
         <v>10</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="67.5" x14ac:dyDescent="0.15">
@@ -3444,7 +3444,7 @@
         <v>56000131</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>68</v>
@@ -3453,7 +3453,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -3464,16 +3464,16 @@
         <v>49</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M23" s="10">
         <v>10</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -3482,10 +3482,10 @@
       </c>
       <c r="B24" s="39"/>
       <c r="C24" s="40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
@@ -3500,16 +3500,16 @@
         <v>49</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M24" s="13">
         <v>0</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
@@ -3517,13 +3517,13 @@
         <v>56000202</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E25" s="30">
         <v>0</v>
@@ -3538,16 +3538,16 @@
         <v>48</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L25" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M25" s="13">
         <v>0</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="33.75" x14ac:dyDescent="0.15">
@@ -3556,16 +3556,16 @@
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E26" s="30">
         <v>0</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="31"/>
@@ -3576,16 +3576,16 @@
         <v>48</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L26" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M26" s="13">
         <v>30</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3616,119 +3616,119 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
         <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
         <v>96</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
         <v>97</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
         <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>